<commit_message>
clean the code + add random portfolios for statistic test
</commit_message>
<xml_diff>
--- a/DATA_PROJECT.xlsx
+++ b/DATA_PROJECT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmona\Mon Drive (guillaume.monarcha.univ@gmail.com)\___DAUPHINE\_AAM_2022\PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCD76EE0-36CC-4496-83E7-69BA368E82FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9DDE34-F757-44C7-BA55-58AFA66133B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1005" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,13 +164,13 @@
     <t>TOTALENERGIES SE</t>
   </si>
   <si>
-    <t>UNILEVER NV</t>
-  </si>
-  <si>
     <t>VIVENDI SE</t>
   </si>
   <si>
     <t>VOLKSWAGEN AG-PREF</t>
+  </si>
+  <si>
+    <t>EUROSTOXX 50 TR index</t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -874,13 +874,13 @@
         <v>2.9469813177973148E-2</v>
       </c>
       <c r="AT2" s="4">
-        <v>1.2681042509841589E-2</v>
+        <v>-2.9718050000619223E-2</v>
       </c>
       <c r="AU2" s="4">
-        <v>-2.9718050000619223E-2</v>
+        <v>-5.4894164953577129E-2</v>
       </c>
       <c r="AV2" s="4">
-        <v>-5.4894164953577129E-2</v>
+        <v>-1.7133128281069498E-2</v>
       </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.25">
@@ -1020,13 +1020,13 @@
         <v>6.569595780652171E-2</v>
       </c>
       <c r="AT3" s="4">
-        <v>6.1719066498550079E-2</v>
+        <v>6.6348473053510215E-2</v>
       </c>
       <c r="AU3" s="4">
-        <v>6.6348473053510215E-2</v>
+        <v>0.17986471305303908</v>
       </c>
       <c r="AV3" s="4">
-        <v>0.17986471305303908</v>
+        <v>5.0471161995195413E-2</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.25">
@@ -1166,13 +1166,13 @@
         <v>-7.7938461725306385E-2</v>
       </c>
       <c r="AT4" s="4">
-        <v>-2.1908012072986649E-2</v>
+        <v>-3.2396658608391693E-2</v>
       </c>
       <c r="AU4" s="4">
-        <v>-3.2396658608391693E-2</v>
+        <v>-0.10743081722782721</v>
       </c>
       <c r="AV4" s="4">
-        <v>-0.10743081722782721</v>
+        <v>-3.0920355900968088E-2</v>
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
@@ -1312,13 +1312,13 @@
         <v>2.8303859407645682E-2</v>
       </c>
       <c r="AT5" s="4">
-        <v>-4.9224592132832701E-3</v>
+        <v>-6.2027680548168984E-2</v>
       </c>
       <c r="AU5" s="4">
-        <v>-6.2027680548168984E-2</v>
+        <v>-3.9810254431557612E-2</v>
       </c>
       <c r="AV5" s="4">
-        <v>-3.9810254431557612E-2</v>
+        <v>3.9494290655950559E-2</v>
       </c>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.25">
@@ -1458,13 +1458,13 @@
         <v>-9.4145676023604796E-4</v>
       </c>
       <c r="AT6" s="4">
-        <v>1.4007884941523718E-2</v>
+        <v>7.3434780315417392E-2</v>
       </c>
       <c r="AU6" s="4">
-        <v>7.3434780315417392E-2</v>
+        <v>-1.5364614111806896E-3</v>
       </c>
       <c r="AV6" s="4">
-        <v>-1.5364614111806896E-3</v>
+        <v>3.8279343806328914E-2</v>
       </c>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
@@ -1604,13 +1604,13 @@
         <v>7.0688616228829382E-2</v>
       </c>
       <c r="AT7" s="4">
-        <v>-8.6014031581915784E-4</v>
+        <v>-2.5698667158036925E-2</v>
       </c>
       <c r="AU7" s="4">
-        <v>-2.5698667158036925E-2</v>
+        <v>9.1074810606060597E-2</v>
       </c>
       <c r="AV7" s="4">
-        <v>9.1074810606060597E-2</v>
+        <v>3.2522901767562118E-2</v>
       </c>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
@@ -1750,13 +1750,13 @@
         <v>-7.130390789182206E-2</v>
       </c>
       <c r="AT8" s="4">
-        <v>6.9131336495693585E-3</v>
+        <v>-1.2797397652339559E-2</v>
       </c>
       <c r="AU8" s="4">
-        <v>-1.2797397652339559E-2</v>
+        <v>0.21938941567036241</v>
       </c>
       <c r="AV8" s="4">
-        <v>0.21938941567036241</v>
+        <v>2.2782684233386474E-2</v>
       </c>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
@@ -1896,13 +1896,13 @@
         <v>3.1754525366389119E-2</v>
       </c>
       <c r="AT9" s="4">
-        <v>-1.1157793831259921E-2</v>
+        <v>0.11355334746736823</v>
       </c>
       <c r="AU9" s="4">
-        <v>0.11355334746736823</v>
+        <v>4.7421616427630875E-2</v>
       </c>
       <c r="AV9" s="4">
-        <v>4.7421616427630875E-2</v>
+        <v>2.1922250092954787E-2</v>
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
@@ -2042,13 +2042,13 @@
         <v>6.890583286078833E-3</v>
       </c>
       <c r="AT10" s="4">
-        <v>-5.2095387396672299E-3</v>
+        <v>2.1172395600362437E-2</v>
       </c>
       <c r="AU10" s="4">
-        <v>2.1172395600362437E-2</v>
+        <v>-2.8489883288313589E-2</v>
       </c>
       <c r="AV10" s="4">
-        <v>-2.8489883288313589E-2</v>
+        <v>-1.102611175342938E-3</v>
       </c>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
@@ -2188,13 +2188,13 @@
         <v>-4.8478031525381771E-2</v>
       </c>
       <c r="AT11" s="4">
-        <v>-5.8693648215618288E-2</v>
+        <v>2.4035491660583386E-3</v>
       </c>
       <c r="AU11" s="4">
-        <v>2.4035491660583386E-3</v>
+        <v>-8.1680830972615692E-2</v>
       </c>
       <c r="AV11" s="4">
-        <v>-8.1680830972615692E-2</v>
+        <v>-4.2522349286764127E-2</v>
       </c>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.25">
@@ -2334,13 +2334,13 @@
         <v>1.679892648614989E-2</v>
       </c>
       <c r="AT12" s="4">
-        <v>1.5957918102583957E-2</v>
+        <v>-2.1075866396262022E-2</v>
       </c>
       <c r="AU12" s="4">
-        <v>-2.1075866396262022E-2</v>
+        <v>5.5984004570122092E-3</v>
       </c>
       <c r="AV12" s="4">
-        <v>5.5984004570122092E-3</v>
+        <v>7.3438679764485926E-3</v>
       </c>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.25">
@@ -2480,13 +2480,13 @@
         <v>3.4986273604269424E-2</v>
       </c>
       <c r="AT13" s="4">
-        <v>4.6548028329990165E-2</v>
+        <v>-3.2483289076092103E-2</v>
       </c>
       <c r="AU13" s="4">
-        <v>-3.2483289076092103E-2</v>
+        <v>6.1788710257721258E-2</v>
       </c>
       <c r="AV13" s="4">
-        <v>6.1788710257721258E-2</v>
+        <v>1.2650244416754441E-2</v>
       </c>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.25">
@@ -2626,13 +2626,13 @@
         <v>-1.0329483727228639E-2</v>
       </c>
       <c r="AT14" s="4">
-        <v>2.1447180287892387E-3</v>
+        <v>1.2823849520880337E-2</v>
       </c>
       <c r="AU14" s="4">
-        <v>1.2823849520880337E-2</v>
+        <v>5.7212155799686082E-2</v>
       </c>
       <c r="AV14" s="4">
-        <v>5.7212155799686082E-2</v>
+        <v>3.3414166425303371E-2</v>
       </c>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.25">
@@ -2772,13 +2772,13 @@
         <v>-1.8026917483213722E-2</v>
       </c>
       <c r="AT15" s="4">
-        <v>3.8504798876104473E-2</v>
+        <v>5.8845515920293412E-2</v>
       </c>
       <c r="AU15" s="4">
-        <v>5.8845515920293412E-2</v>
+        <v>5.2108636977058032E-2</v>
       </c>
       <c r="AV15" s="4">
-        <v>5.2108636977058032E-2</v>
+        <v>2.3910972705623701E-2</v>
       </c>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.25">
@@ -2918,13 +2918,13 @@
         <v>2.5120685147277388E-2</v>
       </c>
       <c r="AT16" s="4">
-        <v>-1.5466372229644421E-3</v>
+        <v>4.3617349865419319E-2</v>
       </c>
       <c r="AU16" s="4">
-        <v>4.3617349865419319E-2</v>
+        <v>0.10931712870175891</v>
       </c>
       <c r="AV16" s="4">
-        <v>0.10931712870175891</v>
+        <v>2.7759042352398122E-2</v>
       </c>
     </row>
     <row r="17" spans="1:48" x14ac:dyDescent="0.25">
@@ -3064,13 +3064,13 @@
         <v>2.5554852264898509E-2</v>
       </c>
       <c r="AT17" s="4">
-        <v>5.4393429061041054E-2</v>
+        <v>-2.0897194681098408E-2</v>
       </c>
       <c r="AU17" s="4">
-        <v>-2.0897194681098408E-2</v>
+        <v>1.25601630364085E-2</v>
       </c>
       <c r="AV17" s="4">
-        <v>1.25601630364085E-2</v>
+        <v>-2.2942926424227572E-3</v>
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.25">
@@ -3210,13 +3210,13 @@
         <v>2.0541640571332342E-2</v>
       </c>
       <c r="AT18" s="4">
-        <v>3.8097106189128649E-2</v>
+        <v>1.9270422869727577E-2</v>
       </c>
       <c r="AU18" s="4">
-        <v>1.9270422869727577E-2</v>
+        <v>7.9193787826881357E-2</v>
       </c>
       <c r="AV18" s="4">
-        <v>7.9193787826881357E-2</v>
+        <v>3.3312338284326337E-2</v>
       </c>
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.25">
@@ -3356,13 +3356,13 @@
         <v>-5.2151081670225308E-2</v>
       </c>
       <c r="AT19" s="4">
-        <v>-1.2555624966258727E-2</v>
+        <v>6.653674243226626E-2</v>
       </c>
       <c r="AU19" s="4">
-        <v>6.653674243226626E-2</v>
+        <v>4.430982487698909E-3</v>
       </c>
       <c r="AV19" s="4">
-        <v>4.430982487698909E-3</v>
+        <v>1.5223455197520108E-2</v>
       </c>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.25">
@@ -3502,13 +3502,13 @@
         <v>-1.5057455047108537E-2</v>
       </c>
       <c r="AT20" s="4">
-        <v>-4.6452141992423868E-2</v>
+        <v>-5.4778739969809975E-2</v>
       </c>
       <c r="AU20" s="4">
-        <v>-5.4778739969809975E-2</v>
+        <v>0.17340233608554234</v>
       </c>
       <c r="AV20" s="4">
-        <v>0.17340233608554234</v>
+        <v>-2.1631241060439788E-2</v>
       </c>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.25">
@@ -3648,13 +3648,13 @@
         <v>2.8028681251343057E-2</v>
       </c>
       <c r="AT21" s="4">
-        <v>0.12666325381386301</v>
+        <v>1.9090144988442859E-2</v>
       </c>
       <c r="AU21" s="4">
-        <v>1.9090144988442859E-2</v>
+        <v>0.15574533987228834</v>
       </c>
       <c r="AV21" s="4">
-        <v>0.15574533987228834</v>
+        <v>2.3415055401238227E-2</v>
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.25">
@@ -3794,13 +3794,13 @@
         <v>3.8322018284705717E-2</v>
       </c>
       <c r="AT22" s="4">
-        <v>2.5946645438253979E-2</v>
+        <v>3.8135200057733742E-2</v>
       </c>
       <c r="AU22" s="4">
-        <v>3.8135200057733742E-2</v>
+        <v>-1.5419721318638557E-2</v>
       </c>
       <c r="AV22" s="4">
-        <v>-1.5419721318638557E-2</v>
+        <v>5.5386128219949926E-2</v>
       </c>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.25">
@@ -3940,13 +3940,13 @@
         <v>4.6577409576125772E-2</v>
       </c>
       <c r="AT23" s="4">
-        <v>-1.3605393971818369E-3</v>
+        <v>6.5831810598236284E-2</v>
       </c>
       <c r="AU23" s="4">
-        <v>6.5831810598236284E-2</v>
+        <v>-1.8245115733207196E-2</v>
       </c>
       <c r="AV23" s="4">
-        <v>-1.8245115733207196E-2</v>
+        <v>3.9764106696549284E-2</v>
       </c>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.25">
@@ -4086,13 +4086,13 @@
         <v>7.6070974690974458E-2</v>
       </c>
       <c r="AT24" s="4">
-        <v>4.2649286695026101E-2</v>
+        <v>-1.4516655019799596E-2</v>
       </c>
       <c r="AU24" s="4">
-        <v>-1.4516655019799596E-2</v>
+        <v>5.4245733171265798E-2</v>
       </c>
       <c r="AV24" s="4">
-        <v>5.4245733171265798E-2</v>
+        <v>-2.6353352900306826E-3</v>
       </c>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.25">
@@ -4232,13 +4232,13 @@
         <v>-3.2856819418570993E-2</v>
       </c>
       <c r="AT25" s="4">
-        <v>-2.5238364219165699E-2</v>
+        <v>-1.8484026208552828E-2</v>
       </c>
       <c r="AU25" s="4">
-        <v>-1.8484026208552828E-2</v>
+        <v>7.6476697761727275E-2</v>
       </c>
       <c r="AV25" s="4">
-        <v>7.6476697761727275E-2</v>
+        <v>-3.7778344382118023E-2</v>
       </c>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.25">
@@ -4378,13 +4378,13 @@
         <v>-5.1990455342584951E-2</v>
       </c>
       <c r="AT26" s="4">
-        <v>-3.5711667556840299E-3</v>
+        <v>-4.1825607829538036E-2</v>
       </c>
       <c r="AU26" s="4">
-        <v>-4.1825607829538036E-2</v>
+        <v>0.10595452010657413</v>
       </c>
       <c r="AV26" s="4">
-        <v>0.10595452010657413</v>
+        <v>-3.5047097494653734E-3</v>
       </c>
     </row>
     <row r="27" spans="1:48" x14ac:dyDescent="0.25">
@@ -4524,13 +4524,13 @@
         <v>3.2035397207733407E-2</v>
       </c>
       <c r="AT27" s="4">
-        <v>-3.1810761005892751E-2</v>
+        <v>-1.3662410777118716E-2</v>
       </c>
       <c r="AU27" s="4">
-        <v>-1.3662410777118716E-2</v>
+        <v>5.0631087776025874E-2</v>
       </c>
       <c r="AV27" s="4">
-        <v>5.0631087776025874E-2</v>
+        <v>2.0293392341029115E-2</v>
       </c>
     </row>
     <row r="28" spans="1:48" x14ac:dyDescent="0.25">
@@ -4670,13 +4670,13 @@
         <v>-2.402654099525936E-2</v>
       </c>
       <c r="AT28" s="4">
-        <v>3.0076929200529623E-2</v>
+        <v>4.9994394104636575E-2</v>
       </c>
       <c r="AU28" s="4">
-        <v>4.9994394104636575E-2</v>
+        <v>0.35751015091148708</v>
       </c>
       <c r="AV28" s="4">
-        <v>0.35751015091148708</v>
+        <v>2.5338076304330048E-2</v>
       </c>
     </row>
     <row r="29" spans="1:48" x14ac:dyDescent="0.25">
@@ -4816,13 +4816,13 @@
         <v>1.0724060461908769E-2</v>
       </c>
       <c r="AT29" s="4">
-        <v>9.6863034390697988E-2</v>
+        <v>9.9790323833190975E-3</v>
       </c>
       <c r="AU29" s="4">
-        <v>9.9790323833190975E-3</v>
+        <v>-0.20847479503251987</v>
       </c>
       <c r="AV29" s="4">
-        <v>-0.20847479503251987</v>
+        <v>-1.9110776232494464E-2</v>
       </c>
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.25">
@@ -4962,13 +4962,13 @@
         <v>2.8969739438308162E-2</v>
       </c>
       <c r="AT30" s="4">
-        <v>3.5184022751437949E-2</v>
+        <v>-3.1717350351789797E-4</v>
       </c>
       <c r="AU30" s="4">
-        <v>-3.1717350351789797E-4</v>
+        <v>-3.5583378825798206E-2</v>
       </c>
       <c r="AV30" s="4">
-        <v>-3.5583378825798206E-2</v>
+        <v>1.1568628963218863E-3</v>
       </c>
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.25">
@@ -5108,13 +5108,13 @@
         <v>-0.14288254755996699</v>
       </c>
       <c r="AT31" s="4">
-        <v>-0.12994771524920345</v>
+        <v>-0.14435973118227885</v>
       </c>
       <c r="AU31" s="4">
-        <v>-0.14435973118227885</v>
+        <v>-7.0999044328456939E-2</v>
       </c>
       <c r="AV31" s="4">
-        <v>-7.0999044328456939E-2</v>
+        <v>-0.13703153045581651</v>
       </c>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.25">
@@ -5254,13 +5254,13 @@
         <v>2.6277315911624077E-2</v>
       </c>
       <c r="AT32" s="4">
-        <v>-6.2042407023507606E-2</v>
+        <v>-2.3472965077082075E-2</v>
       </c>
       <c r="AU32" s="4">
-        <v>-2.3472965077082075E-2</v>
+        <v>-1.0445351818440751E-2</v>
       </c>
       <c r="AV32" s="4">
-        <v>-1.0445351818440751E-2</v>
+        <v>-1.7698182869915757E-2</v>
       </c>
     </row>
     <row r="33" spans="1:48" x14ac:dyDescent="0.25">
@@ -5400,13 +5400,13 @@
         <v>-5.9011959109280698E-2</v>
       </c>
       <c r="AT33" s="4">
-        <v>3.821759882325737E-2</v>
+        <v>-5.6059926127929871E-2</v>
       </c>
       <c r="AU33" s="4">
-        <v>-5.6059926127929871E-2</v>
+        <v>0.14489172504238224</v>
       </c>
       <c r="AV33" s="4">
-        <v>0.14489172504238224</v>
+        <v>-2.5483414243158364E-2</v>
       </c>
     </row>
     <row r="34" spans="1:48" x14ac:dyDescent="0.25">
@@ -5546,13 +5546,13 @@
         <v>0.14668507551179477</v>
       </c>
       <c r="AT34" s="4">
-        <v>2.1708172058716224E-2</v>
+        <v>5.3330895349545937E-2</v>
       </c>
       <c r="AU34" s="4">
-        <v>5.3330895349545937E-2</v>
+        <v>2.5389219883915182E-2</v>
       </c>
       <c r="AV34" s="4">
-        <v>2.5389219883915182E-2</v>
+        <v>6.079115222499909E-2</v>
       </c>
     </row>
     <row r="35" spans="1:48" x14ac:dyDescent="0.25">
@@ -5692,13 +5692,13 @@
         <v>5.939629141727587E-2</v>
       </c>
       <c r="AT35" s="4">
-        <v>1.322349493397823E-4</v>
+        <v>9.0221039231570543E-2</v>
       </c>
       <c r="AU35" s="4">
-        <v>9.0221039231570543E-2</v>
+        <v>-8.0480361838071945E-2</v>
       </c>
       <c r="AV35" s="4">
-        <v>-8.0480361838071945E-2</v>
+        <v>4.3655223946199584E-3</v>
       </c>
     </row>
     <row r="36" spans="1:48" x14ac:dyDescent="0.25">
@@ -5838,13 +5838,13 @@
         <v>-3.3695911467687467E-2</v>
       </c>
       <c r="AT36" s="4">
-        <v>-0.1446816417835779</v>
+        <v>-0.10790183215506455</v>
       </c>
       <c r="AU36" s="4">
-        <v>-0.10790183215506455</v>
+        <v>-5.5714825432806703E-2</v>
       </c>
       <c r="AV36" s="4">
-        <v>-5.5714825432806703E-2</v>
+        <v>-0.11141900857405929</v>
       </c>
     </row>
     <row r="37" spans="1:48" x14ac:dyDescent="0.25">
@@ -5984,13 +5984,13 @@
         <v>-8.8560613369502938E-2</v>
       </c>
       <c r="AT37" s="4">
-        <v>-1.8796427049474929E-2</v>
+        <v>0.11908473245201745</v>
       </c>
       <c r="AU37" s="4">
-        <v>0.11908473245201745</v>
+        <v>9.0727229936455656E-2</v>
       </c>
       <c r="AV37" s="4">
-        <v>9.0727229936455656E-2</v>
+        <v>5.2363137769424473E-3</v>
       </c>
     </row>
     <row r="38" spans="1:48" x14ac:dyDescent="0.25">
@@ -6130,13 +6130,13 @@
         <v>-7.1870213322373644E-3</v>
       </c>
       <c r="AT38" s="4">
-        <v>6.3102765536181993E-2</v>
+        <v>-1.9649331731331432E-2</v>
       </c>
       <c r="AU38" s="4">
-        <v>-1.9649331731331432E-2</v>
+        <v>4.9016434710684287E-2</v>
       </c>
       <c r="AV38" s="4">
-        <v>4.9016434710684287E-2</v>
+        <v>6.6631782968507025E-4</v>
       </c>
     </row>
     <row r="39" spans="1:48" x14ac:dyDescent="0.25">
@@ -6276,13 +6276,13 @@
         <v>-0.13181747625789642</v>
       </c>
       <c r="AT39" s="4">
-        <v>5.140282367077198E-2</v>
+        <v>-0.16716738430168876</v>
       </c>
       <c r="AU39" s="4">
-        <v>-0.16716738430168876</v>
+        <v>-0.1640041138155639</v>
       </c>
       <c r="AV39" s="4">
-        <v>-0.1640041138155639</v>
+        <v>-9.6113057596155071E-2</v>
       </c>
     </row>
     <row r="40" spans="1:48" x14ac:dyDescent="0.25">
@@ -6422,13 +6422,13 @@
         <v>5.519044858493416E-3</v>
       </c>
       <c r="AT40" s="4">
-        <v>-5.3426739654640398E-2</v>
+        <v>-7.3344793457311042E-2</v>
       </c>
       <c r="AU40" s="4">
-        <v>-7.3344793457311042E-2</v>
+        <v>-0.44905273517592059</v>
       </c>
       <c r="AV40" s="4">
-        <v>-0.44905273517592059</v>
+        <v>-0.14663803731493663</v>
       </c>
     </row>
     <row r="41" spans="1:48" x14ac:dyDescent="0.25">
@@ -6568,13 +6568,13 @@
         <v>-1.4300211036774257E-2</v>
       </c>
       <c r="AT41" s="4">
-        <v>-1.2536018415672756E-2</v>
+        <v>9.0421046714261655E-2</v>
       </c>
       <c r="AU41" s="4">
-        <v>9.0421046714261655E-2</v>
+        <v>-0.34020572517379466</v>
       </c>
       <c r="AV41" s="4">
-        <v>-0.34020572517379466</v>
+        <v>-5.775758976064671E-2</v>
       </c>
     </row>
     <row r="42" spans="1:48" x14ac:dyDescent="0.25">
@@ -6714,13 +6714,13 @@
         <v>-5.2130689324050294E-2</v>
       </c>
       <c r="AT42" s="4">
-        <v>-3.3879585440703575E-2</v>
+        <v>4.5611547879881309E-2</v>
       </c>
       <c r="AU42" s="4">
-        <v>4.5611547879881309E-2</v>
+        <v>0.18811903526385843</v>
       </c>
       <c r="AV42" s="4">
-        <v>0.18811903526385843</v>
+        <v>7.4372482181592758E-3</v>
       </c>
     </row>
     <row r="43" spans="1:48" x14ac:dyDescent="0.25">
@@ -6860,13 +6860,13 @@
         <v>6.8108027058668696E-3</v>
       </c>
       <c r="AT43" s="4">
-        <v>-3.0823940334773203E-2</v>
+        <v>-0.1313093961468772</v>
       </c>
       <c r="AU43" s="4">
-        <v>-0.1313093961468772</v>
+        <v>1.9198268168094001E-2</v>
       </c>
       <c r="AV43" s="4">
-        <v>1.9198268168094001E-2</v>
+        <v>-8.437270137616526E-2</v>
       </c>
     </row>
     <row r="44" spans="1:48" x14ac:dyDescent="0.25">
@@ -7006,13 +7006,13 @@
         <v>-4.326715621694488E-2</v>
       </c>
       <c r="AT44" s="4">
-        <v>-0.10679915908230286</v>
+        <v>-6.1609625971962068E-2</v>
       </c>
       <c r="AU44" s="4">
-        <v>-6.1609625971962068E-2</v>
+        <v>-8.076837084513333E-2</v>
       </c>
       <c r="AV44" s="4">
-        <v>-8.076837084513333E-2</v>
+        <v>-0.11587369749445686</v>
       </c>
     </row>
     <row r="45" spans="1:48" x14ac:dyDescent="0.25">
@@ -7152,13 +7152,13 @@
         <v>-1.4688126764920151E-3</v>
       </c>
       <c r="AT45" s="4">
-        <v>-6.5663801337153771E-2</v>
+        <v>5.0624489672483008E-2</v>
       </c>
       <c r="AU45" s="4">
-        <v>5.0624489672483008E-2</v>
+        <v>0.21673389139996346</v>
       </c>
       <c r="AV45" s="4">
-        <v>0.21673389139996346</v>
+        <v>4.8580066412251544E-2</v>
       </c>
     </row>
     <row r="46" spans="1:48" x14ac:dyDescent="0.25">
@@ -7298,13 +7298,13 @@
         <v>2.4582841176858494E-2</v>
       </c>
       <c r="AT46" s="4">
-        <v>0.12762273322311279</v>
+        <v>2.7359603926196741E-2</v>
       </c>
       <c r="AU46" s="4">
-        <v>2.7359603926196741E-2</v>
+        <v>0.15074129601865716</v>
       </c>
       <c r="AV46" s="4">
-        <v>0.15074129601865716</v>
+        <v>0.15487241537947671</v>
       </c>
     </row>
     <row r="47" spans="1:48" x14ac:dyDescent="0.25">
@@ -7444,13 +7444,13 @@
         <v>9.2363390936098577E-2</v>
       </c>
       <c r="AT47" s="4">
-        <v>7.2037445596118577E-2</v>
+        <v>-2.8087920093019303E-2</v>
       </c>
       <c r="AU47" s="4">
-        <v>-2.8087920093019303E-2</v>
+        <v>5.1665484445345244E-2</v>
       </c>
       <c r="AV47" s="4">
-        <v>5.1665484445345244E-2</v>
+        <v>4.9150359610158567E-2</v>
       </c>
     </row>
     <row r="48" spans="1:48" x14ac:dyDescent="0.25">
@@ -7590,13 +7590,13 @@
         <v>-5.570545661688675E-2</v>
       </c>
       <c r="AT48" s="4">
-        <v>1.3982966753242287E-2</v>
+        <v>-8.2663092046470044E-2</v>
       </c>
       <c r="AU48" s="4">
-        <v>-8.2663092046470044E-2</v>
+        <v>-1.426054399295229E-2</v>
       </c>
       <c r="AV48" s="4">
-        <v>-1.426054399295229E-2</v>
+        <v>-1.7978165098485821E-2</v>
       </c>
     </row>
     <row r="49" spans="1:48" x14ac:dyDescent="0.25">
@@ -7736,13 +7736,13 @@
         <v>1.1174272509285155E-2</v>
       </c>
       <c r="AT49" s="4">
-        <v>0.1352718670087607</v>
+        <v>5.8121081658627061E-2</v>
       </c>
       <c r="AU49" s="4">
-        <v>5.8121081658627061E-2</v>
+        <v>0.10510808244428316</v>
       </c>
       <c r="AV49" s="4">
-        <v>0.10510808244428316</v>
+        <v>9.9457375221459143E-2</v>
       </c>
     </row>
     <row r="50" spans="1:48" x14ac:dyDescent="0.25">
@@ -7882,13 +7882,13 @@
         <v>2.7242651665472906E-2</v>
       </c>
       <c r="AT50" s="4">
-        <v>-4.9135168562487452E-3</v>
+        <v>0.10235811232217618</v>
       </c>
       <c r="AU50" s="4">
-        <v>0.10235811232217618</v>
+        <v>0.19057607500726581</v>
       </c>
       <c r="AV50" s="4">
-        <v>0.19057607500726581</v>
+        <v>5.332578613322414E-2</v>
       </c>
     </row>
     <row r="51" spans="1:48" x14ac:dyDescent="0.25">
@@ -8028,13 +8028,13 @@
         <v>1.588625109233921E-2</v>
       </c>
       <c r="AT51" s="4">
-        <v>1.2990388092081417E-2</v>
+        <v>6.4161109988549958E-2</v>
       </c>
       <c r="AU51" s="4">
-        <v>6.4161109988549958E-2</v>
+        <v>0.21567378822130934</v>
       </c>
       <c r="AV51" s="4">
-        <v>0.21567378822130934</v>
+        <v>3.570971223679642E-2</v>
       </c>
     </row>
     <row r="52" spans="1:48" x14ac:dyDescent="0.25">
@@ -8174,13 +8174,13 @@
         <v>7.4013541073036926E-4</v>
       </c>
       <c r="AT52" s="4">
-        <v>7.0767011336553276E-2</v>
+        <v>-0.10545836603458314</v>
       </c>
       <c r="AU52" s="4">
-        <v>-0.10545836603458314</v>
+        <v>-0.14977038990064784</v>
       </c>
       <c r="AV52" s="4">
-        <v>-0.14977038990064784</v>
+        <v>-4.4301421884659464E-2</v>
       </c>
     </row>
     <row r="53" spans="1:48" x14ac:dyDescent="0.25">
@@ -8320,13 +8320,13 @@
         <v>4.1569144316364603E-2</v>
       </c>
       <c r="AT53" s="4">
-        <v>-7.903161959261884E-3</v>
+        <v>1.4532950316272109E-2</v>
       </c>
       <c r="AU53" s="4">
-        <v>1.4532950316272109E-2</v>
+        <v>-0.16506309877088321</v>
       </c>
       <c r="AV53" s="4">
-        <v>-0.16506309877088321</v>
+        <v>2.258493028843378E-2</v>
       </c>
     </row>
     <row r="54" spans="1:48" x14ac:dyDescent="0.25">
@@ -8466,13 +8466,13 @@
         <v>9.2089156029929509E-2</v>
       </c>
       <c r="AT54" s="4">
-        <v>0.11393720905813587</v>
+        <v>8.363321895835063E-2</v>
       </c>
       <c r="AU54" s="4">
-        <v>8.363321895835063E-2</v>
+        <v>0.16354289649744191</v>
       </c>
       <c r="AV54" s="4">
-        <v>0.16354289649744191</v>
+        <v>6.1292589086620497E-2</v>
       </c>
     </row>
     <row r="55" spans="1:48" x14ac:dyDescent="0.25">
@@ -8612,13 +8612,13 @@
         <v>-6.5660254977219501E-2</v>
       </c>
       <c r="AT55" s="4">
-        <v>-1.3828186122797792E-2</v>
+        <v>-9.3525550263869217E-2</v>
       </c>
       <c r="AU55" s="4">
-        <v>-9.3525550263869217E-2</v>
+        <v>-0.10861431138357469</v>
       </c>
       <c r="AV55" s="4">
-        <v>-0.10861431138357469</v>
+        <v>-6.2868139330425454E-2</v>
       </c>
     </row>
     <row r="56" spans="1:48" x14ac:dyDescent="0.25">
@@ -8758,13 +8758,13 @@
         <v>-2.5444533747158715E-2</v>
       </c>
       <c r="AT56" s="4">
-        <v>-1.463700607273255E-2</v>
+        <v>-1.8573213677155476E-2</v>
       </c>
       <c r="AU56" s="4">
-        <v>-1.8573213677155476E-2</v>
+        <v>2.0478098987359861E-2</v>
       </c>
       <c r="AV56" s="4">
-        <v>2.0478098987359861E-2</v>
+        <v>-1.6648191391733347E-2</v>
       </c>
     </row>
     <row r="57" spans="1:48" x14ac:dyDescent="0.25">
@@ -8904,13 +8904,13 @@
         <v>4.8803048483192946E-2</v>
       </c>
       <c r="AT57" s="4">
-        <v>2.0286612258623604E-2</v>
+        <v>7.1083396029862911E-2</v>
       </c>
       <c r="AU57" s="4">
-        <v>7.1083396029862911E-2</v>
+        <v>0.1423292780702059</v>
       </c>
       <c r="AV57" s="4">
-        <v>0.1423292780702059</v>
+        <v>7.4837317711521578E-2</v>
       </c>
     </row>
     <row r="58" spans="1:48" x14ac:dyDescent="0.25">
@@ -9050,13 +9050,13 @@
         <v>-4.6766224924292721E-2</v>
       </c>
       <c r="AT58" s="4">
-        <v>2.5245450684853399E-2</v>
+        <v>-7.5646030609621828E-4</v>
       </c>
       <c r="AU58" s="4">
-        <v>-7.5646030609621828E-4</v>
+        <v>9.2472790153595774E-2</v>
       </c>
       <c r="AV58" s="4">
-        <v>9.2472790153595774E-2</v>
+        <v>-3.6598208452254033E-2</v>
       </c>
     </row>
     <row r="59" spans="1:48" x14ac:dyDescent="0.25">
@@ -9196,13 +9196,13 @@
         <v>-5.1677146671647245E-2</v>
       </c>
       <c r="AT59" s="4">
-        <v>-1.9878951988822502E-2</v>
+        <v>-3.7459613642815692E-2</v>
       </c>
       <c r="AU59" s="4">
-        <v>-3.7459613642815692E-2</v>
+        <v>-1.1163769424865633E-2</v>
       </c>
       <c r="AV59" s="4">
-        <v>-1.1163769424865633E-2</v>
+        <v>-5.7137821878478712E-2</v>
       </c>
     </row>
     <row r="60" spans="1:48" x14ac:dyDescent="0.25">
@@ -9342,13 +9342,13 @@
         <v>-2.0276751488979894E-2</v>
       </c>
       <c r="AT60" s="4">
-        <v>1.2340850960492089E-2</v>
+        <v>-4.6487458217465694E-2</v>
       </c>
       <c r="AU60" s="4">
-        <v>-4.6487458217465694E-2</v>
+        <v>9.0582098265570288E-3</v>
       </c>
       <c r="AV60" s="4">
-        <v>9.0582098265570288E-3</v>
+        <v>-1.1834739526894178E-2</v>
       </c>
     </row>
     <row r="61" spans="1:48" x14ac:dyDescent="0.25">
@@ -9488,13 +9488,13 @@
         <v>4.720768814112053E-2</v>
       </c>
       <c r="AT61" s="4">
-        <v>2.8817097105828804E-3</v>
+        <v>9.693336475578862E-2</v>
       </c>
       <c r="AU61" s="4">
-        <v>9.693336475578862E-2</v>
+        <v>0.12338098615206583</v>
       </c>
       <c r="AV61" s="4">
-        <v>0.12338098615206583</v>
+        <v>6.5999923381188097E-2</v>
       </c>
     </row>
     <row r="62" spans="1:48" x14ac:dyDescent="0.25">
@@ -9634,13 +9634,13 @@
         <v>-4.7532460607353277E-2</v>
       </c>
       <c r="AT62" s="4">
-        <v>-5.7984250500908607E-2</v>
+        <v>-1.8933036133901293E-3</v>
       </c>
       <c r="AU62" s="4">
-        <v>-1.8933036133901293E-3</v>
+        <v>-3.419002209559252E-2</v>
       </c>
       <c r="AV62" s="4">
-        <v>-3.419002209559252E-2</v>
+        <v>-4.2091833869775774E-2</v>
       </c>
     </row>
     <row r="63" spans="1:48" x14ac:dyDescent="0.25">
@@ -9780,13 +9780,13 @@
         <v>2.5359093648936293E-2</v>
       </c>
       <c r="AT63" s="4">
-        <v>4.6674515002522732E-2</v>
+        <v>8.9073346607114079E-2</v>
       </c>
       <c r="AU63" s="4">
-        <v>8.9073346607114079E-2</v>
+        <v>0.12733293196869355</v>
       </c>
       <c r="AV63" s="4">
-        <v>0.12733293196869355</v>
+        <v>4.8319135615754183E-2</v>
       </c>
     </row>
     <row r="64" spans="1:48" x14ac:dyDescent="0.25">
@@ -9926,13 +9926,13 @@
         <v>3.2799953408122917E-2</v>
       </c>
       <c r="AT64" s="4">
-        <v>-3.3726839380850304E-2</v>
+        <v>2.219806554420467E-2</v>
       </c>
       <c r="AU64" s="4">
-        <v>2.219806554420467E-2</v>
+        <v>0.21992752241083346</v>
       </c>
       <c r="AV64" s="4">
-        <v>0.21992752241083346</v>
+        <v>3.6022313480240875E-2</v>
       </c>
     </row>
     <row r="65" spans="1:48" x14ac:dyDescent="0.25">
@@ -10072,13 +10072,13 @@
         <v>-1.6705611182186275E-2</v>
       </c>
       <c r="AT65" s="4">
-        <v>3.0649042380452407E-2</v>
+        <v>-8.2948640483383795E-2</v>
       </c>
       <c r="AU65" s="4">
-        <v>-8.2948640483383795E-2</v>
+        <v>0.14629585621192986</v>
       </c>
       <c r="AV65" s="4">
-        <v>0.14629585621192986</v>
+        <v>-6.481371535161673E-2</v>
       </c>
     </row>
     <row r="66" spans="1:48" x14ac:dyDescent="0.25">
@@ -10218,13 +10218,13 @@
         <v>6.2575941676792146E-2</v>
       </c>
       <c r="AT66" s="4">
-        <v>7.6852748198343424E-2</v>
+        <v>7.4756872150330889E-2</v>
       </c>
       <c r="AU66" s="4">
-        <v>7.4756872150330889E-2</v>
+        <v>-1.938405302926971E-2</v>
       </c>
       <c r="AV66" s="4">
-        <v>-1.938405302926971E-2</v>
+        <v>5.3953662320393114E-2</v>
       </c>
     </row>
     <row r="67" spans="1:48" x14ac:dyDescent="0.25">
@@ -10364,13 +10364,13 @@
         <v>7.730165235591846E-2</v>
       </c>
       <c r="AT67" s="4">
-        <v>-7.0941946173664894E-2</v>
+        <v>3.6378572567098644E-2</v>
       </c>
       <c r="AU67" s="4">
-        <v>3.6378572567098644E-2</v>
+        <v>-2.8006809760656948E-2</v>
       </c>
       <c r="AV67" s="4">
-        <v>-2.8006809760656948E-2</v>
+        <v>5.9618126819395378E-2</v>
       </c>
     </row>
     <row r="68" spans="1:48" x14ac:dyDescent="0.25">
@@ -10510,13 +10510,13 @@
         <v>3.9680998960460068E-2</v>
       </c>
       <c r="AT68" s="4">
-        <v>1.9247856869559099E-2</v>
+        <v>-1.3132054042543251E-2</v>
       </c>
       <c r="AU68" s="4">
-        <v>-1.3132054042543251E-2</v>
+        <v>4.1526432676236791E-2</v>
       </c>
       <c r="AV68" s="4">
-        <v>4.1526432676236791E-2</v>
+        <v>2.0359395316243534E-2</v>
       </c>
     </row>
     <row r="69" spans="1:48" x14ac:dyDescent="0.25">
@@ -10656,13 +10656,13 @@
         <v>-3.2762125615504067E-2</v>
       </c>
       <c r="AT69" s="4">
-        <v>1.0675394781745506E-2</v>
+        <v>-2.4683513954157466E-2</v>
       </c>
       <c r="AU69" s="4">
-        <v>-2.4683513954157466E-2</v>
+        <v>-6.8755736056231198E-2</v>
       </c>
       <c r="AV69" s="4">
-        <v>-6.8755736056231198E-2</v>
+        <v>-3.3763771104889484E-2</v>
       </c>
     </row>
     <row r="70" spans="1:48" x14ac:dyDescent="0.25">
@@ -10802,13 +10802,13 @@
         <v>6.1681402014219788E-3</v>
       </c>
       <c r="AT70" s="4">
-        <v>-2.9222981787819791E-3</v>
+        <v>5.1366200818614205E-2</v>
       </c>
       <c r="AU70" s="4">
-        <v>5.1366200818614205E-2</v>
+        <v>0.16208129735854393</v>
       </c>
       <c r="AV70" s="4">
-        <v>0.16208129735854393</v>
+        <v>3.88728141904644E-2</v>
       </c>
     </row>
     <row r="71" spans="1:48" x14ac:dyDescent="0.25">
@@ -10948,13 +10948,13 @@
         <v>-4.7069836529757936E-2</v>
       </c>
       <c r="AT71" s="4">
-        <v>3.0035188828239745E-2</v>
+        <v>-1.7536475869808998E-2</v>
       </c>
       <c r="AU71" s="4">
-        <v>-1.7536475869808998E-2</v>
+        <v>-5.5647811006667824E-2</v>
       </c>
       <c r="AV71" s="4">
-        <v>-5.5647811006667824E-2</v>
+        <v>-3.3319205618793979E-2</v>
       </c>
     </row>
     <row r="72" spans="1:48" x14ac:dyDescent="0.25">
@@ -11094,13 +11094,13 @@
         <v>-3.7475197848910735E-3</v>
       </c>
       <c r="AT72" s="4">
-        <v>6.8504819547186013E-3</v>
+        <v>-1.1340377933266921E-2</v>
       </c>
       <c r="AU72" s="4">
-        <v>-1.1340377933266921E-2</v>
+        <v>0.15356610865836018</v>
       </c>
       <c r="AV72" s="4">
-        <v>0.15356610865836018</v>
+        <v>-2.8310691043926806E-3</v>
       </c>
     </row>
     <row r="73" spans="1:48" x14ac:dyDescent="0.25">
@@ -11240,13 +11240,13 @@
         <v>-5.2657741791429125E-2</v>
       </c>
       <c r="AT73" s="4">
-        <v>-2.8527579133604819E-3</v>
+        <v>-0.12881094808805638</v>
       </c>
       <c r="AU73" s="4">
-        <v>-0.12881094808805638</v>
+        <v>-2.0371440824926812E-2</v>
       </c>
       <c r="AV73" s="4">
-        <v>-2.0371440824926812E-2</v>
+        <v>-6.1511887189472647E-2</v>
       </c>
     </row>
     <row r="74" spans="1:48" x14ac:dyDescent="0.25">
@@ -11386,13 +11386,13 @@
         <v>-0.10018632033678732</v>
       </c>
       <c r="AT74" s="4">
-        <v>4.5503801658797416E-2</v>
+        <v>1.5570384493168055E-2</v>
       </c>
       <c r="AU74" s="4">
-        <v>1.5570384493168055E-2</v>
+        <v>-0.16851617446917855</v>
       </c>
       <c r="AV74" s="4">
-        <v>-0.16851617446917855</v>
+        <v>-0.13704164770344185</v>
       </c>
     </row>
     <row r="75" spans="1:48" x14ac:dyDescent="0.25">
@@ -11532,13 +11532,13 @@
         <v>-5.024635627878804E-3</v>
       </c>
       <c r="AT75" s="4">
-        <v>-1.0621001107660177E-3</v>
+        <v>-9.6084779887903315E-2</v>
       </c>
       <c r="AU75" s="4">
-        <v>-9.6084779887903315E-2</v>
+        <v>-0.13712922000995809</v>
       </c>
       <c r="AV75" s="4">
-        <v>-0.13712922000995809</v>
+        <v>-5.0766657445923014E-2</v>
       </c>
     </row>
     <row r="76" spans="1:48" x14ac:dyDescent="0.25">
@@ -11678,13 +11678,13 @@
         <v>0.13780493663467186</v>
       </c>
       <c r="AT76" s="4">
-        <v>6.6638541922022343E-2</v>
+        <v>5.9673414101888866E-2</v>
       </c>
       <c r="AU76" s="4">
-        <v>5.9673414101888866E-2</v>
+        <v>0.26736396678428354</v>
       </c>
       <c r="AV76" s="4">
-        <v>0.26736396678428354</v>
+        <v>9.4999074003464523E-2</v>
       </c>
     </row>
     <row r="77" spans="1:48" x14ac:dyDescent="0.25">
@@ -11824,13 +11824,13 @@
         <v>1.3752558654840152E-2</v>
       </c>
       <c r="AT77" s="4">
-        <v>3.7245187014291803E-2</v>
+        <v>5.3529328220423222E-2</v>
       </c>
       <c r="AU77" s="4">
-        <v>5.3529328220423222E-2</v>
+        <v>6.7038930726439627E-3</v>
       </c>
       <c r="AV77" s="4">
-        <v>6.7038930726439627E-3</v>
+        <v>-1.9649150733858423E-2</v>
       </c>
     </row>
     <row r="78" spans="1:48" x14ac:dyDescent="0.25">
@@ -11970,13 +11970,13 @@
         <v>4.6468893846074444E-2</v>
       </c>
       <c r="AT78" s="4">
-        <v>2.8549492055558234E-2</v>
+        <v>-1.1674463122986367E-2</v>
       </c>
       <c r="AU78" s="4">
-        <v>-1.1674463122986367E-2</v>
+        <v>-9.3224303923811092E-2</v>
       </c>
       <c r="AV78" s="4">
-        <v>-9.3224303923811092E-2</v>
+        <v>-5.0538750180767478E-3</v>
       </c>
     </row>
     <row r="79" spans="1:48" x14ac:dyDescent="0.25">
@@ -12116,13 +12116,13 @@
         <v>2.2911943758119335E-2</v>
       </c>
       <c r="AT79" s="4">
-        <v>-3.776420666609881E-2</v>
+        <v>-5.438326081322542E-2</v>
       </c>
       <c r="AU79" s="4">
-        <v>-5.438326081322542E-2</v>
+        <v>0.16933343270404899</v>
       </c>
       <c r="AV79" s="4">
-        <v>0.16933343270404899</v>
+        <v>4.6164712962278198E-2</v>
       </c>
     </row>
     <row r="80" spans="1:48" x14ac:dyDescent="0.25">
@@ -12262,13 +12262,13 @@
         <v>3.9227374030404549E-2</v>
       </c>
       <c r="AT80" s="4">
-        <v>-1.0160411102260181E-2</v>
+        <v>7.5007933531432425E-3</v>
       </c>
       <c r="AU80" s="4">
-        <v>7.5007933531432425E-3</v>
+        <v>3.6942069344210848E-2</v>
       </c>
       <c r="AV80" s="4">
-        <v>3.6942069344210848E-2</v>
+        <v>3.979379181748377E-2</v>
       </c>
     </row>
     <row r="81" spans="1:48" x14ac:dyDescent="0.25">
@@ -12408,13 +12408,13 @@
         <v>-7.7043344650096324E-2</v>
       </c>
       <c r="AT81" s="4">
-        <v>2.6599339881915096E-2</v>
+        <v>-0.14639349425879788</v>
       </c>
       <c r="AU81" s="4">
-        <v>-0.14639349425879788</v>
+        <v>-6.0566516786995761E-2</v>
       </c>
       <c r="AV81" s="4">
-        <v>-6.0566516786995761E-2</v>
+        <v>-1.3110918889521872E-2</v>
       </c>
     </row>
     <row r="82" spans="1:48" x14ac:dyDescent="0.25">
@@ -12554,13 +12554,13 @@
         <v>-5.6747082570712815E-2</v>
       </c>
       <c r="AT82" s="4">
-        <v>1.1494841795419042E-2</v>
+        <v>1.4894080944633625E-2</v>
       </c>
       <c r="AU82" s="4">
-        <v>1.4894080944633625E-2</v>
+        <v>0.11181068281217743</v>
       </c>
       <c r="AV82" s="4">
-        <v>0.11181068281217743</v>
+        <v>-6.2135687105401849E-2</v>
       </c>
     </row>
     <row r="83" spans="1:48" x14ac:dyDescent="0.25">
@@ -12700,13 +12700,13 @@
         <v>-3.6179542182229185E-2</v>
       </c>
       <c r="AT83" s="4">
-        <v>-3.1772685368102183E-2</v>
+        <v>4.0704688558726776E-2</v>
       </c>
       <c r="AU83" s="4">
-        <v>4.0704688558726776E-2</v>
+        <v>-9.7832139025571641E-2</v>
       </c>
       <c r="AV83" s="4">
-        <v>-9.7832139025571641E-2</v>
+        <v>-6.7293251173263013E-2</v>
       </c>
     </row>
     <row r="84" spans="1:48" x14ac:dyDescent="0.25">
@@ -12846,13 +12846,13 @@
         <v>3.7869607043482745E-2</v>
       </c>
       <c r="AT84" s="4">
-        <v>6.1045120078683457E-2</v>
+        <v>0.12021215778441197</v>
       </c>
       <c r="AU84" s="4">
-        <v>0.12021215778441197</v>
+        <v>-3.485752419755439E-2</v>
       </c>
       <c r="AV84" s="4">
-        <v>-3.485752419755439E-2</v>
+        <v>7.2628975015545549E-2</v>
       </c>
     </row>
     <row r="85" spans="1:48" x14ac:dyDescent="0.25">
@@ -12992,13 +12992,13 @@
         <v>5.9295728870920161E-2</v>
       </c>
       <c r="AT85" s="4">
-        <v>7.1535988639837456E-2</v>
+        <v>5.6732159564514717E-2</v>
       </c>
       <c r="AU85" s="4">
-        <v>5.6732159564514717E-2</v>
+        <v>0.11557057447361596</v>
       </c>
       <c r="AV85" s="4">
-        <v>0.11557057447361596</v>
+        <v>2.8712761002086085E-2</v>
       </c>
     </row>
     <row r="86" spans="1:48" x14ac:dyDescent="0.25">
@@ -13138,13 +13138,13 @@
         <v>5.5843439016867169E-2</v>
       </c>
       <c r="AT86" s="4">
-        <v>-1.1809637750348045E-2</v>
+        <v>8.41113972955565E-3</v>
       </c>
       <c r="AU86" s="4">
-        <v>8.41113972955565E-3</v>
+        <v>1.0070836051822241E-2</v>
       </c>
       <c r="AV86" s="4">
-        <v>1.0070836051822241E-2</v>
+        <v>4.9840288612504224E-2</v>
       </c>
     </row>
     <row r="87" spans="1:48" x14ac:dyDescent="0.25">
@@ -13284,13 +13284,13 @@
         <v>-1.416383118410669E-2</v>
       </c>
       <c r="AT87" s="4">
-        <v>-6.1302128927713806E-3</v>
+        <v>-2.6619307977810536E-2</v>
       </c>
       <c r="AU87" s="4">
-        <v>-2.6619307977810536E-2</v>
+        <v>1.1040827531477504E-2</v>
       </c>
       <c r="AV87" s="4">
-        <v>1.1040827531477504E-2</v>
+        <v>7.9416611386016189E-3</v>
       </c>
     </row>
     <row r="88" spans="1:48" x14ac:dyDescent="0.25">
@@ -13430,13 +13430,13 @@
         <v>5.6988943770595046E-3</v>
       </c>
       <c r="AT88" s="4">
-        <v>6.7115037282228229E-3</v>
+        <v>4.0194068607352751E-2</v>
       </c>
       <c r="AU88" s="4">
-        <v>4.0194068607352751E-2</v>
+        <v>0.1243394452709301</v>
       </c>
       <c r="AV88" s="4">
-        <v>0.1243394452709301</v>
+        <v>2.1202374889244036E-2</v>
       </c>
     </row>
     <row r="89" spans="1:48" x14ac:dyDescent="0.25">
@@ -13576,13 +13576,13 @@
         <v>-8.8876000068234262E-3</v>
       </c>
       <c r="AT89" s="4">
-        <v>8.1266986857291723E-2</v>
+        <v>4.6563571625651834E-2</v>
       </c>
       <c r="AU89" s="4">
-        <v>4.6563571625651834E-2</v>
+        <v>4.2917270406402919E-2</v>
       </c>
       <c r="AV89" s="4">
-        <v>4.2917270406402919E-2</v>
+        <v>2.9263338161214847E-2</v>
       </c>
     </row>
     <row r="90" spans="1:48" x14ac:dyDescent="0.25">
@@ -13722,13 +13722,13 @@
         <v>2.9189485213581667E-2</v>
       </c>
       <c r="AT90" s="4">
-        <v>-3.5967615587903623E-2</v>
+        <v>2.6037285794991094E-2</v>
       </c>
       <c r="AU90" s="4">
-        <v>2.6037285794991094E-2</v>
+        <v>3.4243350002918893E-2</v>
       </c>
       <c r="AV90" s="4">
-        <v>3.4243350002918893E-2</v>
+        <v>2.4351389263794321E-2</v>
       </c>
     </row>
     <row r="91" spans="1:48" x14ac:dyDescent="0.25">
@@ -13868,13 +13868,13 @@
         <v>2.3583249082105073E-2</v>
       </c>
       <c r="AT91" s="4">
-        <v>3.5215590851759737E-2</v>
+        <v>-6.8445716942578505E-2</v>
       </c>
       <c r="AU91" s="4">
-        <v>-6.8445716942578505E-2</v>
+        <v>5.8091317534261E-2</v>
       </c>
       <c r="AV91" s="4">
-        <v>5.8091317534261E-2</v>
+        <v>2.7988733659918941E-2</v>
       </c>
     </row>
     <row r="92" spans="1:48" x14ac:dyDescent="0.25">
@@ -14014,13 +14014,13 @@
         <v>-4.0946608106442128E-2</v>
       </c>
       <c r="AT92" s="4">
-        <v>9.5335647898562303E-3</v>
+        <v>2.089709069416168E-2</v>
       </c>
       <c r="AU92" s="4">
-        <v>2.089709069416168E-2</v>
+        <v>-8.1801758229252619E-2</v>
       </c>
       <c r="AV92" s="4">
-        <v>-8.1801758229252619E-2</v>
+        <v>-2.5484840207593562E-2</v>
       </c>
     </row>
     <row r="93" spans="1:48" x14ac:dyDescent="0.25">
@@ -14160,13 +14160,13 @@
         <v>-9.6840788045203796E-3</v>
       </c>
       <c r="AT93" s="4">
-        <v>7.148975437412286E-2</v>
+        <v>-3.087769858219902E-4</v>
       </c>
       <c r="AU93" s="4">
-        <v>-3.087769858219902E-4</v>
+        <v>-7.3244509857081974E-2</v>
       </c>
       <c r="AV93" s="4">
-        <v>-7.3244509857081974E-2</v>
+        <v>-2.8999506253759577E-3</v>
       </c>
     </row>
     <row r="94" spans="1:48" x14ac:dyDescent="0.25">
@@ -14306,13 +14306,13 @@
         <v>2.4494640673332846E-2</v>
       </c>
       <c r="AT94" s="4">
-        <v>3.6103098168132064E-3</v>
+        <v>6.7334174152531512E-2</v>
       </c>
       <c r="AU94" s="4">
-        <v>6.7334174152531512E-2</v>
+        <v>1.6771216863995519E-2</v>
       </c>
       <c r="AV94" s="4">
-        <v>1.6771216863995519E-2</v>
+        <v>4.0464390125763083E-2</v>
       </c>
     </row>
     <row r="95" spans="1:48" x14ac:dyDescent="0.25">
@@ -14452,13 +14452,13 @@
         <v>8.2306913811287519E-3</v>
       </c>
       <c r="AT95" s="4">
-        <v>-9.2207456846037372E-3</v>
+        <v>-6.2845153977861945E-2</v>
       </c>
       <c r="AU95" s="4">
-        <v>-6.2845153977861945E-2</v>
+        <v>9.7791953701724665E-2</v>
       </c>
       <c r="AV95" s="4">
-        <v>9.7791953701724665E-2</v>
+        <v>3.2616398812059799E-2</v>
       </c>
     </row>
     <row r="96" spans="1:48" x14ac:dyDescent="0.25">
@@ -14598,13 +14598,13 @@
         <v>-1.1934879735231441E-2</v>
       </c>
       <c r="AT96" s="4">
-        <v>-3.8208617689278745E-2</v>
+        <v>-4.0876457116389098E-2</v>
       </c>
       <c r="AU96" s="4">
-        <v>-4.0876457116389098E-2</v>
+        <v>-7.9312126521993043E-2</v>
       </c>
       <c r="AV96" s="4">
-        <v>-7.9312126521993043E-2</v>
+        <v>-5.8398391508323155E-2</v>
       </c>
     </row>
     <row r="97" spans="1:48" x14ac:dyDescent="0.25">
@@ -14744,13 +14744,13 @@
         <v>6.9190552513108683E-2</v>
       </c>
       <c r="AT97" s="4">
-        <v>6.7850665999624749E-3</v>
+        <v>0.10378965725400757</v>
       </c>
       <c r="AU97" s="4">
-        <v>0.10378965725400757</v>
+        <v>0.14850285277408393</v>
       </c>
       <c r="AV97" s="4">
-        <v>0.14850285277408393</v>
+        <v>6.5168741062783253E-2</v>
       </c>
     </row>
     <row r="98" spans="1:48" x14ac:dyDescent="0.25">
@@ -14890,13 +14890,13 @@
         <v>4.5261137934543338E-2</v>
       </c>
       <c r="AT98" s="4">
-        <v>-5.3956127001873688E-2</v>
+        <v>-4.4529787802921605E-2</v>
       </c>
       <c r="AU98" s="4">
-        <v>-4.4529787802921605E-2</v>
+        <v>-3.6661969137944395E-2</v>
       </c>
       <c r="AV98" s="4">
-        <v>-3.6661969137944395E-2</v>
+        <v>-1.6625329095228847E-2</v>
       </c>
     </row>
     <row r="99" spans="1:48" x14ac:dyDescent="0.25">
@@ -15036,13 +15036,13 @@
         <v>3.7359036408881829E-2</v>
       </c>
       <c r="AT99" s="4">
-        <v>8.9445751490944136E-3</v>
+        <v>0.10818133251927065</v>
       </c>
       <c r="AU99" s="4">
-        <v>0.10818133251927065</v>
+        <v>1.2489708303928371E-2</v>
       </c>
       <c r="AV99" s="4">
-        <v>1.2489708303928371E-2</v>
+        <v>6.4636129708948609E-2</v>
       </c>
     </row>
     <row r="100" spans="1:48" x14ac:dyDescent="0.25">
@@ -15182,13 +15182,13 @@
         <v>5.5252226068360777E-2</v>
       </c>
       <c r="AT100" s="4">
-        <v>1.4253425073533776E-2</v>
+        <v>9.938822125041602E-2</v>
       </c>
       <c r="AU100" s="4">
-        <v>9.938822125041602E-2</v>
+        <v>7.4318780811872598E-2</v>
       </c>
       <c r="AV100" s="4">
-        <v>7.4318780811872598E-2</v>
+        <v>6.118728988012867E-2</v>
       </c>
     </row>
     <row r="101" spans="1:48" x14ac:dyDescent="0.25">
@@ -15328,13 +15328,13 @@
         <v>-1.4801974431586817E-2</v>
       </c>
       <c r="AT101" s="4">
-        <v>2.5578346518158046E-3</v>
+        <v>0</v>
       </c>
       <c r="AU101" s="4">
-        <v>0</v>
+        <v>4.3269783127318773E-2</v>
       </c>
       <c r="AV101" s="4">
-        <v>4.3269783127318773E-2</v>
+        <v>7.838901542313037E-3</v>
       </c>
     </row>
     <row r="102" spans="1:48" x14ac:dyDescent="0.25">
@@ -15474,13 +15474,13 @@
         <v>1.2519880140708706E-2</v>
       </c>
       <c r="AT102" s="4">
-        <v>8.626666296911889E-3</v>
+        <v>2.4597523543045563E-2</v>
       </c>
       <c r="AU102" s="4">
-        <v>2.4597523543045563E-2</v>
+        <v>4.5316594275423672E-2</v>
       </c>
       <c r="AV102" s="4">
-        <v>4.5316594275423672E-2</v>
+        <v>8.1506983112569209E-3</v>
       </c>
     </row>
     <row r="103" spans="1:48" x14ac:dyDescent="0.25">
@@ -15620,13 +15620,13 @@
         <v>-4.9180286701898557E-2</v>
       </c>
       <c r="AT103" s="4">
-        <v>-5.2343054377642306E-2</v>
+        <v>4.0983105422975674E-2</v>
       </c>
       <c r="AU103" s="4">
-        <v>4.0983105422975674E-2</v>
+        <v>-7.8864685650543831E-2</v>
       </c>
       <c r="AV103" s="4">
-        <v>-7.8864685650543831E-2</v>
+        <v>-2.8677224786991751E-2</v>
       </c>
     </row>
     <row r="104" spans="1:48" x14ac:dyDescent="0.25">
@@ -15766,13 +15766,13 @@
         <v>0.11076923889560897</v>
       </c>
       <c r="AT104" s="4">
-        <v>4.3807496083236197E-2</v>
+        <v>3.8870399373531761E-2</v>
       </c>
       <c r="AU104" s="4">
-        <v>3.8870399373531761E-2</v>
+        <v>5.0525097719977818E-3</v>
       </c>
       <c r="AV104" s="4">
-        <v>5.0525097719977818E-3</v>
+        <v>4.5085604999954176E-2</v>
       </c>
     </row>
     <row r="105" spans="1:48" x14ac:dyDescent="0.25">
@@ -15912,13 +15912,13 @@
         <v>2.5008619152350864E-2</v>
       </c>
       <c r="AT105" s="4">
-        <v>4.2612512641569511E-2</v>
+        <v>-2.3894997691532027E-2</v>
       </c>
       <c r="AU105" s="4">
-        <v>-2.3894997691532027E-2</v>
+        <v>-4.7627016533903221E-3</v>
       </c>
       <c r="AV105" s="4">
-        <v>-4.7627016533903221E-3</v>
+        <v>4.9698795180723732E-3</v>
       </c>
     </row>
     <row r="106" spans="1:48" x14ac:dyDescent="0.25">
@@ -16058,13 +16058,13 @@
         <v>8.1512573852973835E-2</v>
       </c>
       <c r="AT106" s="4">
-        <v>2.2279050023275682E-2</v>
+        <v>-4.3525266663449025E-2</v>
       </c>
       <c r="AU106" s="4">
-        <v>-4.3525266663449025E-2</v>
+        <v>3.1897685273929888E-2</v>
       </c>
       <c r="AV106" s="4">
-        <v>3.1897685273929888E-2</v>
+        <v>1.5261083366151063E-2</v>
       </c>
     </row>
     <row r="107" spans="1:48" x14ac:dyDescent="0.25">
@@ -16204,13 +16204,13 @@
         <v>0</v>
       </c>
       <c r="AT107" s="4">
-        <v>5.8038463621646663E-2</v>
+        <v>-5.1672284681992808E-3</v>
       </c>
       <c r="AU107" s="4">
-        <v>-5.1672284681992808E-3</v>
+        <v>2.6248036448726086E-2</v>
       </c>
       <c r="AV107" s="4">
-        <v>2.6248036448726086E-2</v>
+        <v>2.6992839440062033E-2</v>
       </c>
     </row>
     <row r="108" spans="1:48" x14ac:dyDescent="0.25">
@@ -16350,13 +16350,13 @@
         <v>3.7404084871818233E-2</v>
       </c>
       <c r="AT108" s="4">
-        <v>2.1879722199575902E-3</v>
+        <v>-2.0198023819668398E-2</v>
       </c>
       <c r="AU108" s="4">
-        <v>-2.0198023819668398E-2</v>
+        <v>-1.6411767694730961E-2</v>
       </c>
       <c r="AV108" s="4">
-        <v>-1.6411767694730961E-2</v>
+        <v>-3.1017960669360578E-3</v>
       </c>
     </row>
     <row r="109" spans="1:48" x14ac:dyDescent="0.25">
@@ -16496,13 +16496,13 @@
         <v>-8.8859897678486455E-2</v>
       </c>
       <c r="AT109" s="4">
-        <v>-2.090116405559761E-2</v>
+        <v>5.0360829545572194E-2</v>
       </c>
       <c r="AU109" s="4">
-        <v>5.0360829545572194E-2</v>
+        <v>-8.9936976960429793E-2</v>
       </c>
       <c r="AV109" s="4">
-        <v>-8.9936976960429793E-2</v>
+        <v>-3.3766577760193983E-2</v>
       </c>
     </row>
     <row r="110" spans="1:48" x14ac:dyDescent="0.25">
@@ -16642,13 +16642,13 @@
         <v>4.3668771308792431E-2</v>
       </c>
       <c r="AT110" s="4">
-        <v>1.9200633773561071E-2</v>
+        <v>5.4609796248287212E-2</v>
       </c>
       <c r="AU110" s="4">
-        <v>5.4609796248287212E-2</v>
+        <v>-2.1197564852131534E-2</v>
       </c>
       <c r="AV110" s="4">
-        <v>-2.1197564852131534E-2</v>
+        <v>1.8590650022121569E-2</v>
       </c>
     </row>
     <row r="111" spans="1:48" x14ac:dyDescent="0.25">
@@ -16788,13 +16788,13 @@
         <v>3.7929107682139085E-2</v>
       </c>
       <c r="AT111" s="4">
-        <v>-4.1025874359207348E-3</v>
+        <v>-3.4106947573069646E-2</v>
       </c>
       <c r="AU111" s="4">
-        <v>-3.4106947573069646E-2</v>
+        <v>-3.7753219498581014E-2</v>
       </c>
       <c r="AV111" s="4">
-        <v>-3.7753219498581014E-2</v>
+        <v>1.804013081692446E-2</v>
       </c>
     </row>
     <row r="112" spans="1:48" x14ac:dyDescent="0.25">
@@ -16934,13 +16934,13 @@
         <v>-7.8329304414494039E-2</v>
       </c>
       <c r="AT112" s="4">
-        <v>-1.5366223244268173E-2</v>
+        <v>1.8570129090944354E-2</v>
       </c>
       <c r="AU112" s="4">
-        <v>1.8570129090944354E-2</v>
+        <v>3.4367807865723021E-2</v>
       </c>
       <c r="AV112" s="4">
-        <v>3.4367807865723021E-2</v>
+        <v>-3.3884863076843352E-2</v>
       </c>
     </row>
     <row r="113" spans="1:48" x14ac:dyDescent="0.25">
@@ -17080,13 +17080,13 @@
         <v>-5.12433265377088E-2</v>
       </c>
       <c r="AT113" s="4">
-        <v>6.8251243146262075E-2</v>
+        <v>5.1607019010611932E-2</v>
       </c>
       <c r="AU113" s="4">
-        <v>5.1607019010611932E-2</v>
+        <v>8.9091604304364358E-2</v>
       </c>
       <c r="AV113" s="4">
-        <v>8.9091604304364358E-2</v>
+        <v>4.5443603345231232E-2</v>
       </c>
     </row>
     <row r="114" spans="1:48" x14ac:dyDescent="0.25">
@@ -17226,13 +17226,13 @@
         <v>-4.0258239158686648E-2</v>
       </c>
       <c r="AT114" s="4">
-        <v>-1.3374645725723777E-2</v>
+        <v>1.0253954774187113E-2</v>
       </c>
       <c r="AU114" s="4">
-        <v>1.0253954774187113E-2</v>
+        <v>-2.9692045340554696E-3</v>
       </c>
       <c r="AV114" s="4">
-        <v>-2.9692045340554696E-3</v>
+        <v>-3.0769026884383321E-2</v>
       </c>
     </row>
     <row r="115" spans="1:48" x14ac:dyDescent="0.25">
@@ -17372,13 +17372,13 @@
         <v>7.0084640210464899E-2</v>
       </c>
       <c r="AT115" s="4">
-        <v>0.19041618056014165</v>
+        <v>1.6677993990556583E-2</v>
       </c>
       <c r="AU115" s="4">
-        <v>1.6677993990556583E-2</v>
+        <v>7.3924650045945173E-2</v>
       </c>
       <c r="AV115" s="4">
-        <v>7.3924650045945173E-2</v>
+        <v>6.690651785637991E-2</v>
       </c>
     </row>
     <row r="116" spans="1:48" x14ac:dyDescent="0.25">
@@ -17518,13 +17518,13 @@
         <v>6.0109793091222441E-2</v>
       </c>
       <c r="AT116" s="4">
-        <v>1.5580481175061944E-2</v>
+        <v>3.7074826940161287E-2</v>
       </c>
       <c r="AU116" s="4">
-        <v>3.7074826940161287E-2</v>
+        <v>0.13716605511749536</v>
       </c>
       <c r="AV116" s="4">
-        <v>0.13716605511749536</v>
+        <v>7.4055918402001764E-2</v>
       </c>
     </row>
     <row r="117" spans="1:48" x14ac:dyDescent="0.25">
@@ -17664,13 +17664,13 @@
         <v>-2.8169215519526891E-2</v>
       </c>
       <c r="AT117" s="4">
-        <v>3.0816430574267528E-3</v>
+        <v>6.0048853304383254E-2</v>
       </c>
       <c r="AU117" s="4">
-        <v>6.0048853304383254E-2</v>
+        <v>9.911052893183836E-2</v>
       </c>
       <c r="AV117" s="4">
-        <v>9.911052893183836E-2</v>
+        <v>2.8204558369713695E-2</v>
       </c>
     </row>
     <row r="118" spans="1:48" x14ac:dyDescent="0.25">
@@ -17810,13 +17810,13 @@
         <v>4.7757101812838654E-2</v>
       </c>
       <c r="AT118" s="4">
-        <v>5.5876991960308597E-3</v>
+        <v>1.1649491134865242E-2</v>
       </c>
       <c r="AU118" s="4">
-        <v>1.1649491134865242E-2</v>
+        <v>-6.6167799320407727E-2</v>
       </c>
       <c r="AV118" s="4">
-        <v>-6.6167799320407727E-2</v>
+        <v>-1.8638784163488631E-2</v>
       </c>
     </row>
     <row r="119" spans="1:48" x14ac:dyDescent="0.25">
@@ -17956,13 +17956,13 @@
         <v>-5.1767970067624347E-2</v>
       </c>
       <c r="AT119" s="4">
-        <v>-6.6682812140392844E-3</v>
+        <v>3.4569756406200414E-2</v>
       </c>
       <c r="AU119" s="4">
-        <v>3.4569756406200414E-2</v>
+        <v>-2.4133327268786919E-2</v>
       </c>
       <c r="AV119" s="4">
-        <v>-2.4133327268786919E-2</v>
+        <v>-1.1736534027079193E-3</v>
       </c>
     </row>
     <row r="120" spans="1:48" x14ac:dyDescent="0.25">
@@ -18102,13 +18102,13 @@
         <v>-3.9227974144266708E-2</v>
       </c>
       <c r="AT120" s="4">
-        <v>-3.4340567814936218E-2</v>
+        <v>1.6581174366070206E-2</v>
       </c>
       <c r="AU120" s="4">
-        <v>1.6581174366070206E-2</v>
+        <v>-5.8823206858640731E-2</v>
       </c>
       <c r="AV120" s="4">
-        <v>-5.8823206858640731E-2</v>
+        <v>-3.9298473049727334E-2</v>
       </c>
     </row>
     <row r="121" spans="1:48" x14ac:dyDescent="0.25">
@@ -18248,13 +18248,13 @@
         <v>3.4541769497788755E-2</v>
       </c>
       <c r="AT121" s="4">
-        <v>8.7969025167835335E-2</v>
+        <v>5.7895924199127702E-2</v>
       </c>
       <c r="AU121" s="4">
-        <v>5.7895924199127702E-2</v>
+        <v>-0.12307665417936275</v>
       </c>
       <c r="AV121" s="4">
-        <v>-0.12307665417936275</v>
+        <v>5.2161911114328774E-2</v>
       </c>
     </row>
     <row r="122" spans="1:48" x14ac:dyDescent="0.25">
@@ -18394,13 +18394,13 @@
         <v>-9.4730591503054407E-2</v>
       </c>
       <c r="AT122" s="4">
-        <v>-0.11911210406832184</v>
+        <v>-7.8959901620000106E-2</v>
       </c>
       <c r="AU122" s="4">
-        <v>-7.8959901620000106E-2</v>
+        <v>-7.0723378245502011E-2</v>
       </c>
       <c r="AV122" s="4">
-        <v>-7.0723378245502011E-2</v>
+        <v>-9.1250349543872677E-2</v>
       </c>
     </row>
     <row r="123" spans="1:48" x14ac:dyDescent="0.25">
@@ -18540,13 +18540,13 @@
         <v>6.7620615423580333E-4</v>
       </c>
       <c r="AT123" s="4">
-        <v>9.1321436402254097E-3</v>
+        <v>-4.1506201233300732E-2</v>
       </c>
       <c r="AU123" s="4">
-        <v>-4.1506201233300732E-2</v>
+        <v>-0.42330433041874305</v>
       </c>
       <c r="AV123" s="4">
-        <v>-0.42330433041874305</v>
+        <v>-5.0825994915467354E-2</v>
       </c>
     </row>
     <row r="124" spans="1:48" x14ac:dyDescent="0.25">
@@ -18686,13 +18686,13 @@
         <v>9.8134223533788756E-2</v>
       </c>
       <c r="AT124" s="4">
-        <v>0.14764260546537389</v>
+        <v>3.7151852358828563E-2</v>
       </c>
       <c r="AU124" s="4">
-        <v>3.7151852358828563E-2</v>
+        <v>0.11815826339213764</v>
       </c>
       <c r="AV124" s="4">
-        <v>0.11815826339213764</v>
+        <v>0.10343575068148092</v>
       </c>
     </row>
     <row r="125" spans="1:48" x14ac:dyDescent="0.25">
@@ -18832,13 +18832,13 @@
         <v>6.4672850240209856E-2</v>
       </c>
       <c r="AT125" s="4">
-        <v>1.3440750070997431E-2</v>
+        <v>-9.0577375453197329E-2</v>
       </c>
       <c r="AU125" s="4">
-        <v>-9.0577375453197329E-2</v>
+        <v>0.20356675610351016</v>
       </c>
       <c r="AV125" s="4">
-        <v>0.20356675610351016</v>
+        <v>2.693901534845522E-2</v>
       </c>
     </row>
     <row r="126" spans="1:48" x14ac:dyDescent="0.25">
@@ -18978,13 +18978,13 @@
         <v>-0.10887050075494775</v>
       </c>
       <c r="AT126" s="4">
-        <v>-1.7603856760064929E-2</v>
+        <v>-3.5171589550964111E-3</v>
       </c>
       <c r="AU126" s="4">
-        <v>-3.5171589550964111E-3</v>
+        <v>1.6724318199613952E-2</v>
       </c>
       <c r="AV126" s="4">
-        <v>1.6724318199613952E-2</v>
+        <v>-6.7391040591002871E-2</v>
       </c>
     </row>
     <row r="127" spans="1:48" x14ac:dyDescent="0.25">
@@ -19124,13 +19124,13 @@
         <v>-8.3600645679257068E-3</v>
       </c>
       <c r="AT127" s="4">
-        <v>-1.4716337973402771E-3</v>
+        <v>8.5669248166677647E-3</v>
       </c>
       <c r="AU127" s="4">
-        <v>8.5669248166677647E-3</v>
+        <v>-0.20074748572981793</v>
       </c>
       <c r="AV127" s="4">
-        <v>-0.20074748572981793</v>
+        <v>-6.6661848318396499E-2</v>
       </c>
     </row>
     <row r="128" spans="1:48" x14ac:dyDescent="0.25">
@@ -19270,13 +19270,13 @@
         <v>1.1119058934196957E-2</v>
       </c>
       <c r="AT128" s="4">
-        <v>-2.060339216226903E-2</v>
+        <v>5.4362598532209372E-3</v>
       </c>
       <c r="AU128" s="4">
-        <v>5.4362598532209372E-3</v>
+        <v>7.4818480164602352E-3</v>
       </c>
       <c r="AV128" s="4">
-        <v>7.4818480164602352E-3</v>
+        <v>-3.2136496218476585E-2</v>
       </c>
     </row>
     <row r="129" spans="1:48" x14ac:dyDescent="0.25">
@@ -19416,13 +19416,13 @@
         <v>-1.7492132174620978E-2</v>
       </c>
       <c r="AT129" s="4">
-        <v>-1.898059132958374E-3</v>
+        <v>-3.3978778048121105E-2</v>
       </c>
       <c r="AU129" s="4">
-        <v>-3.3978778048121105E-2</v>
+        <v>3.853792187772509E-2</v>
       </c>
       <c r="AV129" s="4">
-        <v>3.853792187772509E-2</v>
+        <v>2.0795107033639182E-2</v>
       </c>
     </row>
     <row r="130" spans="1:48" x14ac:dyDescent="0.25">
@@ -19562,13 +19562,13 @@
         <v>9.6605241938466868E-2</v>
       </c>
       <c r="AT130" s="4">
-        <v>-1.4769916998271349E-2</v>
+        <v>-4.1339443443583535E-2</v>
       </c>
       <c r="AU130" s="4">
-        <v>-4.1339443443583535E-2</v>
+        <v>0.13052758170501155</v>
       </c>
       <c r="AV130" s="4">
-        <v>0.13052758170501155</v>
+        <v>1.3061365251438861E-2</v>
       </c>
     </row>
     <row r="131" spans="1:48" x14ac:dyDescent="0.25">
@@ -19708,13 +19708,13 @@
         <v>-5.8048543558332222E-3</v>
       </c>
       <c r="AT131" s="4">
-        <v>5.4720817875683725E-2</v>
+        <v>6.3848420438062714E-2</v>
       </c>
       <c r="AU131" s="4">
-        <v>6.3848420438062714E-2</v>
+        <v>6.2474843309757944E-2</v>
       </c>
       <c r="AV131" s="4">
-        <v>6.2474843309757944E-2</v>
+        <v>2.4544602714760888E-2</v>
       </c>
     </row>
     <row r="132" spans="1:48" x14ac:dyDescent="0.25">
@@ -19854,13 +19854,13 @@
         <v>7.5135847285598967E-3</v>
       </c>
       <c r="AT132" s="4">
-        <v>1.9793211517474818E-2</v>
+        <v>-5.2161758905143296E-2</v>
       </c>
       <c r="AU132" s="4">
-        <v>-5.2161758905143296E-2</v>
+        <v>-0.19281558652415098</v>
       </c>
       <c r="AV132" s="4">
-        <v>-0.19281558652415098</v>
+        <v>-6.190857359572155E-2</v>
       </c>
     </row>
     <row r="133" spans="1:48" x14ac:dyDescent="0.25">
@@ -20000,13 +20000,13 @@
         <v>-1.4293266764619172E-2</v>
       </c>
       <c r="AT133" s="4">
-        <v>1.0367862233789493E-2</v>
+        <v>4.0530148821640299E-2</v>
       </c>
       <c r="AU133" s="4">
-        <v>4.0530148821640299E-2</v>
+        <v>0.1615905954396375</v>
       </c>
       <c r="AV133" s="4">
-        <v>0.1615905954396375</v>
+        <v>4.5146944916004683E-2</v>
       </c>
     </row>
     <row r="134" spans="1:48" x14ac:dyDescent="0.25">
@@ -20146,13 +20146,13 @@
         <v>-2.3343866541403191E-4</v>
       </c>
       <c r="AT134" s="4">
-        <v>-8.2504576043800348E-3</v>
+        <v>-1.1659348780593826E-2</v>
       </c>
       <c r="AU134" s="4">
-        <v>-1.1659348780593826E-2</v>
+        <v>-1.0336799776813677E-2</v>
       </c>
       <c r="AV134" s="4">
-        <v>-1.0336799776813677E-2</v>
+        <v>1.1460709927309409E-2</v>
       </c>
     </row>
     <row r="135" spans="1:48" x14ac:dyDescent="0.25">
@@ -20292,13 +20292,13 @@
         <v>1.1913846714581844E-3</v>
       </c>
       <c r="AT135" s="4">
-        <v>-2.1824614440939527E-3</v>
+        <v>3.2804335204180246E-2</v>
       </c>
       <c r="AU135" s="4">
-        <v>3.2804335204180246E-2</v>
+        <v>-6.0641850021142307E-2</v>
       </c>
       <c r="AV135" s="4">
-        <v>-6.0641850021142307E-2</v>
+        <v>-6.0021693772600582E-3</v>
       </c>
     </row>
     <row r="136" spans="1:48" x14ac:dyDescent="0.25">
@@ -20438,13 +20438,13 @@
         <v>3.6755872475586315E-2</v>
       </c>
       <c r="AT136" s="4">
-        <v>-6.3860675600391881E-2</v>
+        <v>2.6183317291721853E-2</v>
       </c>
       <c r="AU136" s="4">
-        <v>2.6183317291721853E-2</v>
+        <v>7.0543068835630773E-2</v>
       </c>
       <c r="AV136" s="4">
-        <v>7.0543068835630773E-2</v>
+        <v>1.8694054878567679E-2</v>
       </c>
     </row>
     <row r="137" spans="1:48" x14ac:dyDescent="0.25">
@@ -20584,13 +20584,13 @@
         <v>2.8248978136230285E-2</v>
       </c>
       <c r="AT137" s="4">
-        <v>-7.067956155805688E-3</v>
+        <v>-2.3348854968168187E-2</v>
       </c>
       <c r="AU137" s="4">
-        <v>-2.3348854968168187E-2</v>
+        <v>-2.7157259818468282E-2</v>
       </c>
       <c r="AV137" s="4">
-        <v>-2.7157259818468282E-2</v>
+        <v>9.6927239395139253E-5</v>
       </c>
     </row>
     <row r="138" spans="1:48" x14ac:dyDescent="0.25">
@@ -20730,13 +20730,13 @@
         <v>9.7639554824671348E-2</v>
       </c>
       <c r="AT138" s="4">
-        <v>2.9528558691018114E-2</v>
+        <v>3.6119798748979193E-3</v>
       </c>
       <c r="AU138" s="4">
-        <v>3.6119798748979193E-3</v>
+        <v>9.4829770427300231E-2</v>
       </c>
       <c r="AV138" s="4">
-        <v>9.4829770427300231E-2</v>
+        <v>7.9048199918121176E-2</v>
       </c>
     </row>
     <row r="139" spans="1:48" x14ac:dyDescent="0.25">
@@ -20876,13 +20876,13 @@
         <v>-4.2282249816248618E-2</v>
       </c>
       <c r="AT139" s="4">
-        <v>-4.0076568470709728E-2</v>
+        <v>-6.1750035989804219E-2</v>
       </c>
       <c r="AU139" s="4">
-        <v>-6.1750035989804219E-2</v>
+        <v>7.9115144639818391E-2</v>
       </c>
       <c r="AV139" s="4">
-        <v>7.9115144639818391E-2</v>
+        <v>-1.7206322560863296E-2</v>
       </c>
     </row>
     <row r="140" spans="1:48" x14ac:dyDescent="0.25">
@@ -21022,13 +21022,13 @@
         <v>8.3587628949701731E-3</v>
       </c>
       <c r="AT140" s="4">
-        <v>0.19554719066717463</v>
+        <v>-1.6823560204698773E-2</v>
       </c>
       <c r="AU140" s="4">
-        <v>-1.6823560204698773E-2</v>
+        <v>-2.9187166225137728E-2</v>
       </c>
       <c r="AV140" s="4">
-        <v>-2.9187166225137728E-2</v>
+        <v>2.8783247195260264E-2</v>
       </c>
     </row>
     <row r="141" spans="1:48" x14ac:dyDescent="0.25">
@@ -21168,13 +21168,13 @@
         <v>2.1106242978008893E-2</v>
       </c>
       <c r="AT141" s="4">
-        <v>4.2632409477033839E-2</v>
+        <v>9.4259774356714621E-2</v>
       </c>
       <c r="AU141" s="4">
-        <v>9.4259774356714621E-2</v>
+        <v>-2.2190073158371182E-2</v>
       </c>
       <c r="AV141" s="4">
-        <v>-2.2190073158371182E-2</v>
+        <v>5.6465928531934884E-2</v>
       </c>
     </row>
     <row r="142" spans="1:48" x14ac:dyDescent="0.25">
@@ -21314,13 +21314,13 @@
         <v>-5.1672478711353165E-3</v>
       </c>
       <c r="AT142" s="4">
-        <v>3.3444018506912476E-2</v>
+        <v>-5.4529743877984593E-4</v>
       </c>
       <c r="AU142" s="4">
-        <v>-5.4529743877984593E-4</v>
+        <v>6.5516111027437818E-2</v>
       </c>
       <c r="AV142" s="4">
-        <v>6.5516111027437818E-2</v>
+        <v>1.9620919315601837E-2</v>
       </c>
     </row>
     <row r="143" spans="1:48" x14ac:dyDescent="0.25">
@@ -21460,13 +21460,13 @@
         <v>2.1198534833384297E-3</v>
       </c>
       <c r="AT143" s="4">
-        <v>6.8996345117392277E-2</v>
+        <v>8.3434058554928692E-2</v>
       </c>
       <c r="AU143" s="4">
-        <v>8.3434058554928692E-2</v>
+        <v>-6.7865101273821837E-2</v>
       </c>
       <c r="AV143" s="4">
-        <v>-6.7865101273821837E-2</v>
+        <v>9.8363732532547044E-3</v>
       </c>
     </row>
     <row r="144" spans="1:48" x14ac:dyDescent="0.25">
@@ -21606,13 +21606,13 @@
         <v>-7.1910685729713375E-2</v>
       </c>
       <c r="AT144" s="4">
-        <v>-4.5848243485542617E-2</v>
+        <v>9.5835011930955893E-3</v>
       </c>
       <c r="AU144" s="4">
-        <v>9.5835011930955893E-3</v>
+        <v>-2.9882432697624361E-3</v>
       </c>
       <c r="AV144" s="4">
-        <v>-2.9882432697624361E-3</v>
+        <v>-2.9737013288727798E-2</v>
       </c>
     </row>
     <row r="145" spans="1:48" x14ac:dyDescent="0.25">
@@ -21752,13 +21752,13 @@
         <v>-7.5080690963996721E-3</v>
       </c>
       <c r="AT145" s="4">
-        <v>1.051790328576474E-2</v>
+        <v>4.105499835012516E-3</v>
       </c>
       <c r="AU145" s="4">
-        <v>4.105499835012516E-3</v>
+        <v>-2.4375732524536842E-2</v>
       </c>
       <c r="AV145" s="4">
-        <v>-2.4375732524536842E-2</v>
+        <v>2.9081157325578921E-3</v>
       </c>
     </row>
     <row r="146" spans="1:48" x14ac:dyDescent="0.25">
@@ -21898,13 +21898,13 @@
         <v>1.1289323402880136E-2</v>
       </c>
       <c r="AT146" s="4">
-        <v>2.8454429375798007E-2</v>
+        <v>-1.50709219858155E-2</v>
       </c>
       <c r="AU146" s="4">
-        <v>-1.50709219858155E-2</v>
+        <v>-3.6507361538426264E-2</v>
       </c>
       <c r="AV146" s="4">
-        <v>-3.6507361538426264E-2</v>
+        <v>-7.2202688428760764E-3</v>
       </c>
     </row>
     <row r="147" spans="1:48" x14ac:dyDescent="0.25">
@@ -22044,13 +22044,13 @@
         <v>6.0247832632287501E-2</v>
       </c>
       <c r="AT147" s="4">
-        <v>-2.5990277710929988E-3</v>
+        <v>0.11128526645768022</v>
       </c>
       <c r="AU147" s="4">
-        <v>0.11128526645768022</v>
+        <v>0.10091799877219443</v>
       </c>
       <c r="AV147" s="4">
-        <v>0.10091799877219443</v>
+        <v>5.1536174430128812E-2</v>
       </c>
     </row>
     <row r="148" spans="1:48" x14ac:dyDescent="0.25">
@@ -22190,13 +22190,13 @@
         <v>5.3361704258142018E-2</v>
       </c>
       <c r="AT148" s="4">
-        <v>-8.0170035051096988E-4</v>
+        <v>-4.4407825831948022E-3</v>
       </c>
       <c r="AU148" s="4">
-        <v>-4.4407825831948022E-3</v>
+        <v>0.12970687784487578</v>
       </c>
       <c r="AV148" s="4">
-        <v>0.12970687784487578</v>
+        <v>2.2657592726063047E-2</v>
       </c>
     </row>
     <row r="149" spans="1:48" x14ac:dyDescent="0.25">
@@ -22336,13 +22336,13 @@
         <v>-9.7141922837810091E-3</v>
       </c>
       <c r="AT149" s="4">
-        <v>-2.0168349466183511E-2</v>
+        <v>4.8771934746321355E-2</v>
       </c>
       <c r="AU149" s="4">
-        <v>4.8771934746321355E-2</v>
+        <v>0.14239906942217684</v>
       </c>
       <c r="AV149" s="4">
-        <v>0.14239906942217684</v>
+        <v>-2.7692128371555991E-2</v>
       </c>
     </row>
     <row r="150" spans="1:48" x14ac:dyDescent="0.25">
@@ -22482,13 +22482,13 @@
         <v>-1.5640073837505652E-2</v>
       </c>
       <c r="AT150" s="4">
-        <v>-2.6185552690359382E-2</v>
+        <v>2.4609458591910993E-3</v>
       </c>
       <c r="AU150" s="4">
-        <v>2.4609458591910993E-3</v>
+        <v>-6.5411075904849292E-2</v>
       </c>
       <c r="AV150" s="4">
-        <v>-6.5411075904849292E-2</v>
+        <v>-1.7484091748618202E-2</v>
       </c>
     </row>
     <row r="151" spans="1:48" x14ac:dyDescent="0.25">
@@ -22628,13 +22628,13 @@
         <v>1.2813836603104534E-2</v>
       </c>
       <c r="AT151" s="4">
-        <v>-1.3339008201718738E-2</v>
+        <v>5.396787277190751E-2</v>
       </c>
       <c r="AU151" s="4">
-        <v>5.396787277190751E-2</v>
+        <v>6.3502359969752176E-2</v>
       </c>
       <c r="AV151" s="4">
-        <v>6.3502359969752176E-2</v>
+        <v>3.0907197539341569E-2</v>
       </c>
     </row>
     <row r="152" spans="1:48" x14ac:dyDescent="0.25">
@@ -22774,13 +22774,13 @@
         <v>7.1837503394012181E-3</v>
       </c>
       <c r="AT152" s="4">
-        <v>-6.746730338310003E-2</v>
+        <v>-0.10071901464612587</v>
       </c>
       <c r="AU152" s="4">
-        <v>-0.10071901464612587</v>
+        <v>-8.9820318923800602E-2</v>
       </c>
       <c r="AV152" s="4">
-        <v>-8.9820318923800602E-2</v>
+        <v>-4.6094542391868276E-2</v>
       </c>
     </row>
     <row r="153" spans="1:48" x14ac:dyDescent="0.25">
@@ -22920,13 +22920,13 @@
         <v>-4.7024296045619085E-3</v>
       </c>
       <c r="AT153" s="4">
-        <v>7.4245028848618055E-2</v>
+        <v>-1.1767935191897561E-2</v>
       </c>
       <c r="AU153" s="4">
-        <v>-1.1767935191897561E-2</v>
+        <v>1.61425281568639E-3</v>
       </c>
       <c r="AV153" s="4">
-        <v>1.61425281568639E-3</v>
+        <v>-2.1764628655270402E-2</v>
       </c>
     </row>
     <row r="154" spans="1:48" x14ac:dyDescent="0.25">
@@ -23066,13 +23066,13 @@
         <v>0.13440222987198602</v>
       </c>
       <c r="AT154" s="4">
-        <v>2.159904381839528E-2</v>
+        <v>6.4625486970208312E-2</v>
       </c>
       <c r="AU154" s="4">
-        <v>6.4625486970208312E-2</v>
+        <v>6.481351421284165E-2</v>
       </c>
       <c r="AV154" s="4">
-        <v>6.481351421284165E-2</v>
+        <v>5.806444001020572E-2</v>
       </c>
     </row>
     <row r="155" spans="1:48" x14ac:dyDescent="0.25">
@@ -23212,13 +23212,13 @@
         <v>-5.3502468530575165E-3</v>
       </c>
       <c r="AT155" s="4">
-        <v>1.9132841958966029E-2</v>
+        <v>-1.6904932333442479E-2</v>
       </c>
       <c r="AU155" s="4">
-        <v>-1.6904932333442479E-2</v>
+        <v>-4.1955954232392845E-2</v>
       </c>
       <c r="AV155" s="4">
-        <v>-4.1955954232392845E-2</v>
+        <v>-2.5195559693794944E-2</v>
       </c>
     </row>
     <row r="156" spans="1:48" x14ac:dyDescent="0.25">
@@ -23358,13 +23358,13 @@
         <v>1.4856803331437796E-2</v>
       </c>
       <c r="AT156" s="4">
-        <v>-6.2765130979594019E-3</v>
+        <v>-2.4163695255722817E-2</v>
       </c>
       <c r="AU156" s="4">
-        <v>-2.4163695255722817E-2</v>
+        <v>-0.1163172426787642</v>
       </c>
       <c r="AV156" s="4">
-        <v>-0.1163172426787642</v>
+        <v>-2.021871675493947E-3</v>
       </c>
     </row>
     <row r="157" spans="1:48" x14ac:dyDescent="0.25">
@@ -23504,13 +23504,13 @@
         <v>6.9910191318410142E-2</v>
       </c>
       <c r="AT157" s="4">
-        <v>3.1579657813923578E-2</v>
+        <v>5.7145845681810137E-2</v>
       </c>
       <c r="AU157" s="4">
-        <v>5.7145845681810137E-2</v>
+        <v>7.0314133764151521E-2</v>
       </c>
       <c r="AV157" s="4">
-        <v>7.0314133764151521E-2</v>
+        <v>3.9334439448776237E-2</v>
       </c>
     </row>
     <row r="158" spans="1:48" x14ac:dyDescent="0.25">
@@ -23650,13 +23650,13 @@
         <v>-3.562468836923427E-2</v>
       </c>
       <c r="AT158" s="4">
-        <v>1.199916254481681E-2</v>
+        <v>6.7546174142478765E-3</v>
       </c>
       <c r="AU158" s="4">
-        <v>6.7546174142478765E-3</v>
+        <v>-7.475912268939755E-2</v>
       </c>
       <c r="AV158" s="4">
-        <v>-7.475912268939755E-2</v>
+        <v>-3.7093098756394771E-2</v>
       </c>
     </row>
     <row r="159" spans="1:48" x14ac:dyDescent="0.25">
@@ -23796,13 +23796,13 @@
         <v>4.8503097698005204E-2</v>
       </c>
       <c r="AT159" s="4">
-        <v>-2.6422632824318781E-2</v>
+        <v>-8.0524688122444177E-3</v>
       </c>
       <c r="AU159" s="4">
-        <v>-8.0524688122444177E-3</v>
+        <v>7.6398176480574342E-2</v>
       </c>
       <c r="AV159" s="4">
-        <v>7.6398176480574342E-2</v>
+        <v>2.7416519204448431E-3</v>
       </c>
     </row>
     <row r="160" spans="1:48" x14ac:dyDescent="0.25">
@@ -23942,13 +23942,13 @@
         <v>-6.9484427855797781E-2</v>
       </c>
       <c r="AT160" s="4">
-        <v>-4.1757696896450591E-3</v>
+        <v>-3.7438488721556196E-2</v>
       </c>
       <c r="AU160" s="4">
-        <v>-3.7438488721556196E-2</v>
+        <v>-1.873350720489908E-2</v>
       </c>
       <c r="AV160" s="4">
-        <v>-1.873350720489908E-2</v>
+        <v>-5.8675126606405836E-2</v>
       </c>
     </row>
     <row r="161" spans="1:48" x14ac:dyDescent="0.25">
@@ -24088,13 +24088,13 @@
         <v>-5.3790686513041641E-2</v>
       </c>
       <c r="AT161" s="4">
-        <v>3.1417924298684063E-2</v>
+        <v>3.0927693563993053E-2</v>
       </c>
       <c r="AU161" s="4">
-        <v>3.0927693563993053E-2</v>
+        <v>9.4083703134550944E-4</v>
       </c>
       <c r="AV161" s="4">
-        <v>9.4083703134550944E-4</v>
+        <v>-7.0756541377787752E-3</v>
       </c>
     </row>
     <row r="162" spans="1:48" x14ac:dyDescent="0.25">
@@ -24234,13 +24234,13 @@
         <v>-4.7856850373592774E-2</v>
       </c>
       <c r="AT162" s="4">
-        <v>-2.8688356776956137E-2</v>
+        <v>-3.2728942849155285E-2</v>
       </c>
       <c r="AU162" s="4">
-        <v>-3.2728942849155285E-2</v>
+        <v>-6.7026459668196758E-2</v>
       </c>
       <c r="AV162" s="4">
-        <v>-6.7026459668196758E-2</v>
+        <v>-5.2775732542259979E-2</v>
       </c>
     </row>
     <row r="163" spans="1:48" x14ac:dyDescent="0.25">
@@ -24380,13 +24380,13 @@
         <v>3.8978070731163772E-2</v>
       </c>
       <c r="AT163" s="4">
-        <v>-1.8986751984096162E-2</v>
+        <v>4.5115162025090028E-2</v>
       </c>
       <c r="AU163" s="4">
-        <v>4.5115162025090028E-2</v>
+        <v>6.9826797303310428E-2</v>
       </c>
       <c r="AV163" s="4">
-        <v>6.9826797303310428E-2</v>
+        <v>5.5037260780307351E-2</v>
       </c>
     </row>
     <row r="164" spans="1:48" x14ac:dyDescent="0.25">
@@ -24526,13 +24526,13 @@
         <v>4.1891802875927864E-2</v>
       </c>
       <c r="AT164" s="4">
-        <v>2.745891396953315E-2</v>
+        <v>0.15557735739729917</v>
       </c>
       <c r="AU164" s="4">
-        <v>0.15557735739729917</v>
+        <v>1.5338314001852149E-2</v>
       </c>
       <c r="AV164" s="4">
-        <v>1.5338314001852149E-2</v>
+        <v>4.4167302286550081E-2</v>
       </c>
     </row>
     <row r="165" spans="1:48" x14ac:dyDescent="0.25">
@@ -24672,13 +24672,13 @@
         <v>2.8988726606318238E-3</v>
       </c>
       <c r="AT165" s="4">
-        <v>8.8608110413445074E-2</v>
+        <v>5.0541022558274751E-3</v>
       </c>
       <c r="AU165" s="4">
-        <v>5.0541022558274751E-3</v>
+        <v>-7.0111029096347699E-2</v>
       </c>
       <c r="AV165" s="4">
-        <v>-7.0111029096347699E-2</v>
+        <v>1.8226879340430324E-2</v>
       </c>
     </row>
     <row r="166" spans="1:48" x14ac:dyDescent="0.25">
@@ -24818,13 +24818,13 @@
         <v>5.0517613864831112E-4</v>
       </c>
       <c r="AT166" s="4">
-        <v>4.6511298735306017E-2</v>
+        <v>2.0936798421661296E-2</v>
       </c>
       <c r="AU166" s="4">
-        <v>2.0936798421661296E-2</v>
+        <v>0.10490443398069149</v>
       </c>
       <c r="AV166" s="4">
-        <v>0.10490443398069149</v>
+        <v>5.3293519062974859E-2</v>
       </c>
     </row>
     <row r="167" spans="1:48" x14ac:dyDescent="0.25">
@@ -24964,13 +24964,13 @@
         <v>-5.8633852190105751E-2</v>
       </c>
       <c r="AT167" s="4">
-        <v>3.9532526903276466E-3</v>
+        <v>-6.7258622508759802E-2</v>
       </c>
       <c r="AU167" s="4">
-        <v>-6.7258622508759802E-2</v>
+        <v>-7.0909234524808129E-2</v>
       </c>
       <c r="AV167" s="4">
-        <v>-7.0909234524808129E-2</v>
+        <v>-5.5267856167898755E-2</v>
       </c>
     </row>
     <row r="168" spans="1:48" x14ac:dyDescent="0.25">
@@ -25110,13 +25110,13 @@
         <v>7.0505138031746295E-2</v>
       </c>
       <c r="AT168" s="4">
-        <v>-7.4346437462290416E-3</v>
+        <v>3.3160880876828003E-3</v>
       </c>
       <c r="AU168" s="4">
-        <v>3.3160880876828003E-3</v>
+        <v>6.2507843843746747E-2</v>
       </c>
       <c r="AV168" s="4">
-        <v>6.2507843843746747E-2</v>
+        <v>6.001811769567178E-2</v>
       </c>
     </row>
     <row r="169" spans="1:48" x14ac:dyDescent="0.25">
@@ -25256,13 +25256,13 @@
         <v>-4.5459845478940997E-2</v>
       </c>
       <c r="AT169" s="4">
-        <v>-2.0037558303109271E-2</v>
+        <v>4.0065034475392558E-2</v>
       </c>
       <c r="AU169" s="4">
-        <v>4.0065034475392558E-2</v>
+        <v>1.8350231854569632E-2</v>
       </c>
       <c r="AV169" s="4">
-        <v>1.8350231854569632E-2</v>
+        <v>-8.8866838766654688E-4</v>
       </c>
     </row>
     <row r="170" spans="1:48" x14ac:dyDescent="0.25">
@@ -25402,13 +25402,13 @@
         <v>-3.4973998096881953E-2</v>
       </c>
       <c r="AT170" s="4">
-        <v>8.7248156154314138E-2</v>
+        <v>9.9270872556738166E-3</v>
       </c>
       <c r="AU170" s="4">
-        <v>9.9270872556738166E-3</v>
+        <v>-3.2065552915645501E-2</v>
       </c>
       <c r="AV170" s="4">
-        <v>-3.2065552915645501E-2</v>
+        <v>-1.073353068769356E-2</v>
       </c>
     </row>
     <row r="171" spans="1:48" x14ac:dyDescent="0.25">
@@ -25548,13 +25548,13 @@
         <v>6.9599179610608575E-2</v>
       </c>
       <c r="AT171" s="4">
-        <v>-2.2856544902796649E-2</v>
+        <v>-9.8295088635054206E-3</v>
       </c>
       <c r="AU171" s="4">
-        <v>-9.8295088635054206E-3</v>
+        <v>6.8172944973810878E-2</v>
       </c>
       <c r="AV171" s="4">
-        <v>6.8172944973810878E-2</v>
+        <v>4.2532565137169298E-2</v>
       </c>
     </row>
     <row r="172" spans="1:48" x14ac:dyDescent="0.25">
@@ -25694,13 +25694,13 @@
         <v>-1.566257207836097E-2</v>
       </c>
       <c r="AT172" s="4">
-        <v>-3.2449113762797244E-2</v>
+        <v>-8.7346957404808023E-3</v>
       </c>
       <c r="AU172" s="4">
-        <v>-8.7346957404808023E-3</v>
+        <v>9.3811407333958208E-2</v>
       </c>
       <c r="AV172" s="4">
-        <v>9.3811407333958208E-2</v>
+        <v>1.0798870377841441E-2</v>
       </c>
     </row>
     <row r="173" spans="1:48" x14ac:dyDescent="0.25">
@@ -25840,13 +25840,13 @@
         <v>1.0714148809752189E-2</v>
       </c>
       <c r="AT173" s="4">
-        <v>1.6052626513445301E-2</v>
+        <v>-1.6057831214351115E-3</v>
       </c>
       <c r="AU173" s="4">
-        <v>-1.6057831214351115E-3</v>
+        <v>2.8002937926379756E-2</v>
       </c>
       <c r="AV173" s="4">
-        <v>2.8002937926379756E-2</v>
+        <v>2.7966326820376031E-2</v>
       </c>
     </row>
     <row r="174" spans="1:48" x14ac:dyDescent="0.25">
@@ -25986,13 +25986,13 @@
         <v>3.2745581083433839E-2</v>
       </c>
       <c r="AT174" s="4">
-        <v>-4.7769297877520045E-2</v>
+        <v>3.611617128231126E-2</v>
       </c>
       <c r="AU174" s="4">
-        <v>3.611617128231126E-2</v>
+        <v>4.3319022393295548E-3</v>
       </c>
       <c r="AV174" s="4">
-        <v>4.3319022393295548E-3</v>
+        <v>1.1996842936069507E-2</v>
       </c>
     </row>
     <row r="175" spans="1:48" x14ac:dyDescent="0.25">
@@ -26132,13 +26132,13 @@
         <v>-9.1003785112447444E-2</v>
       </c>
       <c r="AT175" s="4">
-        <v>2.869381230297563E-2</v>
+        <v>-4.1049779394991437E-2</v>
       </c>
       <c r="AU175" s="4">
-        <v>-4.1049779394991437E-2</v>
+        <v>-7.864412428219858E-2</v>
       </c>
       <c r="AV175" s="4">
-        <v>-7.864412428219858E-2</v>
+        <v>-2.6628878791995714E-2</v>
       </c>
     </row>
     <row r="176" spans="1:48" x14ac:dyDescent="0.25">
@@ -26278,13 +26278,13 @@
         <v>-0.13059255409601844</v>
       </c>
       <c r="AT176" s="4">
-        <v>-8.9629383220805381E-2</v>
+        <v>-7.0279365263554716E-2</v>
       </c>
       <c r="AU176" s="4">
-        <v>-7.0279365263554716E-2</v>
+        <v>-8.4984801163041412E-2</v>
       </c>
       <c r="AV176" s="4">
-        <v>-8.4984801163041412E-2</v>
+        <v>-8.458958768149194E-2</v>
       </c>
     </row>
     <row r="177" spans="1:48" x14ac:dyDescent="0.25">
@@ -26424,13 +26424,13 @@
         <v>-5.9226534974695211E-2</v>
       </c>
       <c r="AT177" s="4">
-        <v>-5.9014666033585184E-2</v>
+        <v>-0.15182037168782214</v>
       </c>
       <c r="AU177" s="4">
-        <v>-0.15182037168782214</v>
+        <v>-0.28092608148635234</v>
       </c>
       <c r="AV177" s="4">
-        <v>-0.28092608148635234</v>
+        <v>-0.16210435666487844</v>
       </c>
     </row>
     <row r="178" spans="1:48" x14ac:dyDescent="0.25">
@@ -26570,13 +26570,13 @@
         <v>-7.1772171935287954E-2</v>
       </c>
       <c r="AT178" s="4">
-        <v>1.7297139870567912E-2</v>
+        <v>3.8826022337654642E-2</v>
       </c>
       <c r="AU178" s="4">
-        <v>3.8826022337654642E-2</v>
+        <v>0.2001120631782598</v>
       </c>
       <c r="AV178" s="4">
-        <v>0.2001120631782598</v>
+        <v>5.3243810181714091E-2</v>
       </c>
     </row>
     <row r="179" spans="1:48" x14ac:dyDescent="0.25">
@@ -26716,13 +26716,13 @@
         <v>2.3592116529841167E-2</v>
       </c>
       <c r="AT179" s="4">
-        <v>2.9403279212420808E-2</v>
+        <v>3.6794129937460562E-2</v>
       </c>
       <c r="AU179" s="4">
-        <v>3.6794129937460562E-2</v>
+        <v>3.3377966489895883E-2</v>
       </c>
       <c r="AV179" s="4">
-        <v>3.3377966489895883E-2</v>
+        <v>4.7365608942980142E-2</v>
       </c>
     </row>
     <row r="180" spans="1:48" x14ac:dyDescent="0.25">
@@ -26862,13 +26862,13 @@
         <v>3.0295941045736408E-2</v>
       </c>
       <c r="AT180" s="4">
-        <v>1.6347055589690518E-2</v>
+        <v>0.11796210020083886</v>
       </c>
       <c r="AU180" s="4">
-        <v>0.11796210020083886</v>
+        <v>1.8417485742538764E-2</v>
       </c>
       <c r="AV180" s="4">
-        <v>1.8417485742538764E-2</v>
+        <v>6.3950513574401402E-2</v>
       </c>
     </row>
     <row r="181" spans="1:48" x14ac:dyDescent="0.25">
@@ -27008,13 +27008,13 @@
         <v>-7.8734667290525584E-2</v>
       </c>
       <c r="AT181" s="4">
-        <v>5.9894681578821718E-2</v>
+        <v>-1.9266256858982977E-2</v>
       </c>
       <c r="AU181" s="4">
-        <v>-1.9266256858982977E-2</v>
+        <v>-7.3664385711595171E-2</v>
       </c>
       <c r="AV181" s="4">
-        <v>-7.3664385711595171E-2</v>
+        <v>-1.6053804577982889E-2</v>
       </c>
     </row>
     <row r="182" spans="1:48" x14ac:dyDescent="0.25">
@@ -27154,13 +27154,13 @@
         <v>5.750769292052138E-2</v>
       </c>
       <c r="AT182" s="4">
-        <v>-2.3381735908266199E-2</v>
+        <v>6.2504283462408328E-2</v>
       </c>
       <c r="AU182" s="4">
-        <v>6.2504283462408328E-2</v>
+        <v>0.11472254601642762</v>
       </c>
       <c r="AV182" s="4">
-        <v>0.11472254601642762</v>
+        <v>3.1839244133455624E-2</v>
       </c>
     </row>
     <row r="183" spans="1:48" x14ac:dyDescent="0.25">
@@ -27300,13 +27300,13 @@
         <v>-9.7074396080674918E-2</v>
       </c>
       <c r="AT183" s="4">
-        <v>6.1636684252751817E-2</v>
+        <v>0</v>
       </c>
       <c r="AU183" s="4">
-        <v>0</v>
+        <v>-1.3922326791663608E-2</v>
       </c>
       <c r="AV183" s="4">
-        <v>-1.3922326791663608E-2</v>
+        <v>-2.3266665252709484E-2</v>
       </c>
     </row>
     <row r="184" spans="1:48" x14ac:dyDescent="0.25">
@@ -27446,13 +27446,13 @@
         <v>-0.11575405506175473</v>
       </c>
       <c r="AT184" s="4">
-        <v>-4.939408328797168E-2</v>
+        <v>4.1593122738707411E-2</v>
       </c>
       <c r="AU184" s="4">
-        <v>4.1593122738707411E-2</v>
+        <v>-5.6574225926976363E-2</v>
       </c>
       <c r="AV184" s="4">
-        <v>-5.6574225926976363E-2</v>
+        <v>-7.3097078664697945E-2</v>
       </c>
     </row>
     <row r="185" spans="1:48" x14ac:dyDescent="0.25">
@@ -27592,13 +27592,13 @@
         <v>0.38749032472079903</v>
       </c>
       <c r="AT185" s="4">
-        <v>3.522150632831722E-2</v>
+        <v>1.5735309020076027E-2</v>
       </c>
       <c r="AU185" s="4">
-        <v>1.5735309020076027E-2</v>
+        <v>0.12981914981679732</v>
       </c>
       <c r="AV185" s="4">
-        <v>0.12981914981679732</v>
+        <v>0.18085824147334173</v>
       </c>
     </row>
     <row r="186" spans="1:48" x14ac:dyDescent="0.25">
@@ -27738,13 +27738,13 @@
         <v>-1.4654128147912004E-2</v>
       </c>
       <c r="AT186" s="4">
-        <v>0</v>
+        <v>4.7655206433840913E-2</v>
       </c>
       <c r="AU186" s="4">
-        <v>4.7655206433840913E-2</v>
+        <v>7.8392281470284209E-2</v>
       </c>
       <c r="AV186" s="4">
-        <v>7.8392281470284209E-2</v>
+        <v>1.7720182994814149E-2</v>
       </c>
     </row>
     <row r="187" spans="1:48" x14ac:dyDescent="0.25">
@@ -27884,13 +27884,13 @@
         <v>7.3912794979882346E-3</v>
       </c>
       <c r="AT187" s="4">
-        <v>0</v>
+        <v>-4.0181145810738728E-2</v>
       </c>
       <c r="AU187" s="4">
-        <v>-4.0181145810738728E-2</v>
+        <v>2.6371968117631539E-2</v>
       </c>
       <c r="AV187" s="4">
-        <v>2.6371968117631539E-2</v>
+        <v>-1.8828177287406489E-2</v>
       </c>
     </row>
     <row r="188" spans="1:48" x14ac:dyDescent="0.25">
@@ -28030,13 +28030,13 @@
         <v>9.9727777700465481E-2</v>
       </c>
       <c r="AT188" s="4">
-        <v>0</v>
+        <v>0.1283567774936063</v>
       </c>
       <c r="AU188" s="4">
-        <v>0.1283567774936063</v>
+        <v>0.10598269158409623</v>
       </c>
       <c r="AV188" s="4">
-        <v>0.10598269158409623</v>
+        <v>4.5443889181016495E-2</v>
       </c>
     </row>
     <row r="189" spans="1:48" x14ac:dyDescent="0.25">
@@ -28176,13 +28176,13 @@
         <v>5.4137687684033819E-2</v>
       </c>
       <c r="AT189" s="4">
-        <v>0</v>
+        <v>-1.9950075960744718E-2</v>
       </c>
       <c r="AU189" s="4">
-        <v>-1.9950075960744718E-2</v>
+        <v>0.37903215644767041</v>
       </c>
       <c r="AV189" s="4">
-        <v>0.37903215644767041</v>
+        <v>7.8812173210170311E-2</v>
       </c>
     </row>
     <row r="190" spans="1:48" x14ac:dyDescent="0.25">
@@ -28322,13 +28322,13 @@
         <v>-7.4166483523586679E-2</v>
       </c>
       <c r="AT190" s="4">
-        <v>0</v>
+        <v>3.5713039620788756E-2</v>
       </c>
       <c r="AU190" s="4">
-        <v>3.5713039620788756E-2</v>
+        <v>-9.1785431195762213E-2</v>
       </c>
       <c r="AV190" s="4">
-        <v>-9.1785431195762213E-2</v>
+        <v>1.8222836030881373E-2</v>
       </c>
     </row>
     <row r="191" spans="1:48" x14ac:dyDescent="0.25">
@@ -28468,13 +28468,13 @@
         <v>2.9327045831737397E-2</v>
       </c>
       <c r="AT191" s="4">
-        <v>0</v>
+        <v>2.4827712327712526E-2</v>
       </c>
       <c r="AU191" s="4">
-        <v>2.4827712327712526E-2</v>
+        <v>5.3992806660127401E-2</v>
       </c>
       <c r="AV191" s="4">
-        <v>5.3992806660127401E-2</v>
+        <v>2.3014171350274726E-2</v>
       </c>
     </row>
     <row r="192" spans="1:48" x14ac:dyDescent="0.25">
@@ -28614,13 +28614,13 @@
         <v>2.3099179479626475E-2</v>
       </c>
       <c r="AT192" s="4">
-        <v>0</v>
+        <v>-2.633469671426758E-2</v>
       </c>
       <c r="AU192" s="4">
-        <v>-2.633469671426758E-2</v>
+        <v>-7.5307177782497403E-2</v>
       </c>
       <c r="AV192" s="4">
-        <v>-7.5307177782497403E-2</v>
+        <v>6.8434077239185598E-3</v>
       </c>
     </row>
     <row r="193" spans="1:48" x14ac:dyDescent="0.25">
@@ -28760,13 +28760,13 @@
         <v>-3.8133590688978813E-2</v>
       </c>
       <c r="AT193" s="4">
-        <v>0</v>
+        <v>5.9997202702766206E-3</v>
       </c>
       <c r="AU193" s="4">
-        <v>5.9997202702766206E-3</v>
+        <v>-4.3174304965948318E-3</v>
       </c>
       <c r="AV193" s="4">
-        <v>-4.3174304965948318E-3</v>
+        <v>7.2044834864595231E-3</v>
       </c>
     </row>
     <row r="194" spans="1:48" x14ac:dyDescent="0.25">
@@ -28906,13 +28906,13 @@
         <v>1.7574780696788084E-2</v>
       </c>
       <c r="AT194" s="4">
-        <v>0</v>
+        <v>0.13403519874201164</v>
       </c>
       <c r="AU194" s="4">
-        <v>0.13403519874201164</v>
+        <v>-2.0439265368326742E-2</v>
       </c>
       <c r="AV194" s="4">
-        <v>-2.0439265368326742E-2</v>
+        <v>2.6320499750413839E-2</v>
       </c>
     </row>
     <row r="195" spans="1:48" x14ac:dyDescent="0.25">
@@ -29052,13 +29052,13 @@
         <v>0.12601746380093126</v>
       </c>
       <c r="AT195" s="4">
-        <v>0</v>
+        <v>0.16055296032467403</v>
       </c>
       <c r="AU195" s="4">
-        <v>0.16055296032467403</v>
+        <v>-3.8053659311001797E-2</v>
       </c>
       <c r="AV195" s="4">
-        <v>-3.8053659311001797E-2</v>
+        <v>-3.4101199786820025E-2</v>
       </c>
     </row>
     <row r="196" spans="1:48" x14ac:dyDescent="0.25">
@@ -29198,13 +29198,13 @@
         <v>4.9232395364725123E-2</v>
       </c>
       <c r="AT196" s="4">
-        <v>0</v>
+        <v>2.109112897644283E-2</v>
       </c>
       <c r="AU196" s="4">
-        <v>2.109112897644283E-2</v>
+        <v>9.2970035042561072E-4</v>
       </c>
       <c r="AV196" s="4">
-        <v>9.2970035042561072E-4</v>
+        <v>5.1491393241768657E-2</v>
       </c>
     </row>
     <row r="197" spans="1:48" x14ac:dyDescent="0.25">
@@ -29344,13 +29344,13 @@
         <v>-6.3638433515482706E-2</v>
       </c>
       <c r="AT197" s="4">
-        <v>0</v>
+        <v>1.0327740775490035E-2</v>
       </c>
       <c r="AU197" s="4">
-        <v>1.0327740775490035E-2</v>
+        <v>-0.1659265284586805</v>
       </c>
       <c r="AV197" s="4">
-        <v>-0.1659265284586805</v>
+        <v>-4.3291520770650904E-2</v>
       </c>
     </row>
     <row r="198" spans="1:48" x14ac:dyDescent="0.25">
@@ -29490,13 +29490,13 @@
         <v>9.8990181714810443E-2</v>
       </c>
       <c r="AT198" s="4">
-        <v>0</v>
+        <v>5.6887517301771107E-2</v>
       </c>
       <c r="AU198" s="4">
-        <v>5.6887517301771107E-2</v>
+        <v>9.7859750392071509E-2</v>
       </c>
       <c r="AV198" s="4">
-        <v>9.7859750392071509E-2</v>
+        <v>5.8085388408340322E-2</v>
       </c>
     </row>
     <row r="199" spans="1:48" x14ac:dyDescent="0.25">
@@ -29636,13 +29636,13 @@
         <v>0.14175914960268932</v>
       </c>
       <c r="AT199" s="4">
-        <v>0</v>
+        <v>-2.4388695672509897E-2</v>
       </c>
       <c r="AU199" s="4">
-        <v>-2.4388695672509897E-2</v>
+        <v>3.2906385609420719E-2</v>
       </c>
       <c r="AV199" s="4">
-        <v>3.2906385609420719E-2</v>
+        <v>-2.7781816649282032E-2</v>
       </c>
     </row>
     <row r="200" spans="1:48" x14ac:dyDescent="0.25">
@@ -29782,13 +29782,13 @@
         <v>-9.2194057973135957E-2</v>
       </c>
       <c r="AT200" s="4">
-        <v>0</v>
+        <v>-2.5001797828223427E-2</v>
       </c>
       <c r="AU200" s="4">
-        <v>-2.5001797828223427E-2</v>
+        <v>-2.8804444147444763E-2</v>
       </c>
       <c r="AV200" s="4">
-        <v>-2.8804444147444763E-2</v>
+        <v>-5.9218069622928193E-2</v>
       </c>
     </row>
     <row r="201" spans="1:48" x14ac:dyDescent="0.25">
@@ -29928,13 +29928,13 @@
         <v>2.4144150785185836E-2</v>
       </c>
       <c r="AT201" s="4">
-        <v>0</v>
+        <v>4.6860402222550057E-2</v>
       </c>
       <c r="AU201" s="4">
-        <v>4.6860402222550057E-2</v>
+        <v>-0.11817428478261527</v>
       </c>
       <c r="AV201" s="4">
-        <v>-0.11817428478261527</v>
+        <v>-4.5547800423683116E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>